<commit_message>
spleen updated to latest version fixing layers
</commit_message>
<xml_diff>
--- a/models/spleen/source/spleen.xlsx
+++ b/models/spleen/source/spleen.xlsx
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="565">
   <si>
     <t>id</t>
   </si>
@@ -1460,7 +1460,7 @@
     <t>ns_pals</t>
   </si>
   <si>
-    <t>0, 0, 0, 1, 2, 3, 4, 5, 6, 0</t>
+    <t>0, 0, 1, 2, 3, 4, 5, 6, 0</t>
   </si>
   <si>
     <t>cg-smg, n-splenic, spln, spln, spln, spln, spln, spln, pals</t>
@@ -1482,6 +1482,9 @@
   </si>
   <si>
     <t>ns_nts-dmv</t>
+  </si>
+  <si>
+    <t>0,0,0</t>
   </si>
   <si>
     <t>nts, med, dmv</t>
@@ -2676,15 +2679,15 @@
         <v>7</v>
       </c>
       <c r="F1" s="131" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>123</v>
@@ -2693,37 +2696,37 @@
         <v>73</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="2" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
   </sheetData>
@@ -2747,98 +2750,98 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="132" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B2" s="133" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="132" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B3" s="134" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="132" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B4" s="135" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="132" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B5" s="135" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="132" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B6" s="135" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="132" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B7" s="135" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="132" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="B8" s="135" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="132" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B9" s="135" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="132" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B10" s="135" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="132" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B11" s="135" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B12" s="128" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
   </sheetData>
@@ -2881,97 +2884,97 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="137" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="137" t="s">
+        <v>550</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>549</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="137" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="137" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="B5" s="138" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="137" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B6" s="138" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="137" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B7" s="138" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="139"/>
       <c r="B8" s="138" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="139"/>
       <c r="B9" s="138" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="139"/>
       <c r="B10" s="138" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="139"/>
       <c r="B11" s="138" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="139"/>
       <c r="B12" s="138" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="13">
@@ -9580,11 +9583,11 @@
       <c r="H25" s="104"/>
       <c r="I25" s="101"/>
       <c r="J25" s="101"/>
-      <c r="K25" s="105">
-        <v>0.0</v>
+      <c r="K25" s="105" t="s">
+        <v>471</v>
       </c>
       <c r="L25" s="103" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="M25" s="101"/>
       <c r="N25" s="101"/>
@@ -9596,10 +9599,10 @@
     </row>
     <row r="26">
       <c r="A26" s="106" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B26" s="107" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C26" s="108" t="s">
         <v>420</v>
@@ -9612,7 +9615,7 @@
         <v>367</v>
       </c>
       <c r="G26" s="112" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="H26" s="113"/>
       <c r="I26" s="114"/>
@@ -9621,7 +9624,7 @@
         <v>82</v>
       </c>
       <c r="L26" s="116" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="M26" s="114"/>
       <c r="N26" s="114"/>
@@ -9633,10 +9636,10 @@
     </row>
     <row r="27">
       <c r="A27" s="117" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B27" s="107" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C27" s="108" t="s">
         <v>423</v>
@@ -9649,7 +9652,7 @@
         <v>368</v>
       </c>
       <c r="G27" s="117" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="H27" s="118"/>
       <c r="I27" s="114"/>
@@ -9658,7 +9661,7 @@
         <v>74</v>
       </c>
       <c r="L27" s="116" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="M27" s="114"/>
       <c r="N27" s="114"/>
@@ -9711,13 +9714,13 @@
         <v>383</v>
       </c>
       <c r="D1" s="119" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="G1" s="119" t="s">
         <v>340</v>
@@ -9729,10 +9732,10 @@
         <v>4</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="2">
@@ -9740,13 +9743,13 @@
         <v>147</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C2" s="120"/>
       <c r="D2" s="13"/>
       <c r="G2" s="121"/>
       <c r="I2" s="2" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="3">
@@ -9754,13 +9757,13 @@
         <v>152</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C3" s="121"/>
       <c r="D3" s="13"/>
       <c r="G3" s="121"/>
       <c r="I3" s="2" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="4" ht="20.25" customHeight="1">
@@ -9768,14 +9771,14 @@
         <v>154</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="C4" s="121"/>
       <c r="D4" s="13"/>
       <c r="E4" s="122"/>
       <c r="G4" s="123"/>
       <c r="I4" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="K4" s="124"/>
     </row>
@@ -9784,7 +9787,7 @@
         <v>156</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C5" s="121"/>
       <c r="D5" s="13"/>
@@ -9792,7 +9795,7 @@
       <c r="F5" s="123"/>
       <c r="G5" s="123"/>
       <c r="I5" s="2" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="K5" s="124"/>
     </row>
@@ -9801,21 +9804,21 @@
         <v>158</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="125"/>
       <c r="G6" s="121"/>
       <c r="I6" s="2" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="7" ht="22.5" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>73</v>
@@ -9826,13 +9829,13 @@
     </row>
     <row r="8" ht="22.5" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="125"/>
@@ -9860,16 +9863,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
   </sheetData>
@@ -9899,42 +9902,42 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="127" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C2" s="128" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="129" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C3" s="128" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="130" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="C4" s="128" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="130" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C5" s="128" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
spleen fix incorrect layer for nts dmv
</commit_message>
<xml_diff>
--- a/models/spleen/source/spleen.xlsx
+++ b/models/spleen/source/spleen.xlsx
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="625">
   <si>
     <t>id</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>nts, dmv</t>
+  </si>
+  <si>
+    <t>2,2</t>
   </si>
   <si>
     <t>dmv</t>
@@ -1624,7 +1627,7 @@
     <t>ilxtr:neuron-type-splen-1</t>
   </si>
   <si>
-    <t>preganglionic sympathetic neuron</t>
+    <t>pre-ganglionic sympathetic neuron</t>
   </si>
   <si>
     <t>Neuron population 2 with a soma in the dorsal motor nucleus of the vagus</t>
@@ -1633,7 +1636,7 @@
     <t>ilxtr:neuron-type-splen-2</t>
   </si>
   <si>
-    <t xml:space="preserve">preganglionic parasympathetic neuron </t>
+    <t xml:space="preserve">pre-ganglionic parasympathetic neuron </t>
   </si>
   <si>
     <t xml:space="preserve">Neuron population 3 with a soma in the nucleus tractus solitarius </t>
@@ -1660,7 +1663,7 @@
     <t>ilxtr:neuron-type-splen-5</t>
   </si>
   <si>
-    <t>sympathetic postganglionic neuron</t>
+    <t>sympathetic post-ganglionic neuron</t>
   </si>
   <si>
     <t>col-spl</t>
@@ -2985,60 +2988,60 @@
         <v>5</v>
       </c>
       <c r="D1" s="155" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E1" s="155" t="s">
         <v>8</v>
       </c>
       <c r="F1" s="155" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="2" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="39" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
   </sheetData>
@@ -3062,106 +3065,106 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="157" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="B2" s="158" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="157" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B3" s="159" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="157" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B4" s="160" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="157" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="B5" s="160" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="157" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B6" s="160" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="157" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="B7" s="160" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="157" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="B8" s="160" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="157" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="B9" s="160" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="157" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="B10" s="160" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="157" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B11" s="160" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="B12" s="152" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B13" s="161" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
   </sheetData>
@@ -3205,97 +3208,97 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="163" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="163" t="s">
+        <v>610</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>609</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>610</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="163" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="163" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B5" s="164" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="163" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="B6" s="164" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="163" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="B7" s="164" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="165"/>
       <c r="B8" s="164" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="165"/>
       <c r="B9" s="164" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="165"/>
       <c r="B10" s="164" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="165"/>
       <c r="B11" s="164" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="165"/>
       <c r="B12" s="164" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="13">
@@ -6551,7 +6554,9 @@
       <c r="M7" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="N7" s="21"/>
+      <c r="N7" s="21" t="s">
+        <v>47</v>
+      </c>
       <c r="O7" s="15"/>
       <c r="P7" s="15"/>
       <c r="Q7" s="15"/>
@@ -6560,13 +6565,13 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -6578,7 +6583,7 @@
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
       <c r="M8" s="13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N8" s="16"/>
       <c r="O8" s="15"/>
@@ -6589,13 +6594,13 @@
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -6607,7 +6612,7 @@
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
       <c r="M9" s="13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="N9" s="16"/>
       <c r="O9" s="15"/>
@@ -6618,13 +6623,13 @@
     </row>
     <row r="10">
       <c r="A10" s="13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -6636,7 +6641,7 @@
       <c r="K10" s="15"/>
       <c r="L10" s="15"/>
       <c r="M10" s="21" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="N10" s="21"/>
       <c r="O10" s="15"/>
@@ -6647,13 +6652,13 @@
     </row>
     <row r="11">
       <c r="A11" s="13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
@@ -6665,7 +6670,7 @@
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
       <c r="M11" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N11" s="16"/>
       <c r="O11" s="15"/>
@@ -6676,13 +6681,13 @@
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
@@ -6694,7 +6699,7 @@
       <c r="K12" s="15"/>
       <c r="L12" s="15"/>
       <c r="M12" s="13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N12" s="16"/>
       <c r="O12" s="15"/>
@@ -6705,23 +6710,23 @@
     </row>
     <row r="13">
       <c r="A13" s="13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="13" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
       <c r="I13" s="22" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J13" s="20"/>
       <c r="K13" s="15"/>
@@ -6735,18 +6740,18 @@
     </row>
     <row r="14">
       <c r="A14" s="13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
       <c r="F14" s="23" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
@@ -6754,10 +6759,10 @@
       <c r="K14" s="15"/>
       <c r="L14" s="15"/>
       <c r="M14" s="12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N14" s="21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="O14" s="15"/>
       <c r="P14" s="15"/>
@@ -6767,18 +6772,18 @@
     </row>
     <row r="15">
       <c r="A15" s="13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="23" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
@@ -6787,10 +6792,10 @@
       <c r="K15" s="15"/>
       <c r="L15" s="15"/>
       <c r="M15" s="12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N15" s="21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="O15" s="15"/>
       <c r="P15" s="15"/>
@@ -6800,18 +6805,18 @@
     </row>
     <row r="16">
       <c r="A16" s="24" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D16" s="26"/>
       <c r="E16" s="26"/>
       <c r="F16" s="27" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G16" s="26"/>
       <c r="H16" s="26"/>
@@ -6820,10 +6825,10 @@
       <c r="K16" s="26"/>
       <c r="L16" s="26"/>
       <c r="M16" s="29" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="N16" s="30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="O16" s="26"/>
       <c r="P16" s="26"/>
@@ -6833,13 +6838,13 @@
     </row>
     <row r="17">
       <c r="A17" s="13" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
@@ -6851,7 +6856,7 @@
       <c r="K17" s="15"/>
       <c r="L17" s="15"/>
       <c r="M17" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="N17" s="21"/>
       <c r="O17" s="15"/>
@@ -6862,18 +6867,18 @@
     </row>
     <row r="18">
       <c r="A18" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
       <c r="F18" s="23" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
@@ -6882,10 +6887,10 @@
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
       <c r="M18" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="N18" s="21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="O18" s="15"/>
       <c r="P18" s="15"/>
@@ -6895,13 +6900,13 @@
     </row>
     <row r="19">
       <c r="A19" s="13" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
@@ -6913,7 +6918,7 @@
       <c r="K19" s="15"/>
       <c r="L19" s="15"/>
       <c r="M19" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="N19" s="21"/>
       <c r="O19" s="15"/>
@@ -6924,18 +6929,18 @@
     </row>
     <row r="20">
       <c r="A20" s="13" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="13" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
@@ -6944,10 +6949,10 @@
       <c r="K20" s="15"/>
       <c r="L20" s="15"/>
       <c r="M20" s="12" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="N20" s="21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="O20" s="15"/>
       <c r="P20" s="15"/>
@@ -6957,13 +6962,13 @@
     </row>
     <row r="21">
       <c r="A21" s="13" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="31"/>
@@ -6984,13 +6989,13 @@
     </row>
     <row r="22">
       <c r="A22" s="18" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="31"/>
@@ -6998,7 +7003,7 @@
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
       <c r="I22" s="12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J22" s="20"/>
       <c r="K22" s="15"/>
@@ -7013,13 +7018,13 @@
     </row>
     <row r="23">
       <c r="A23" s="33" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C23" s="35" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D23" s="36"/>
       <c r="E23" s="15"/>
@@ -7040,13 +7045,13 @@
     </row>
     <row r="24">
       <c r="A24" s="33" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B24" s="37" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C24" s="35" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D24" s="36"/>
       <c r="E24" s="15"/>
@@ -7067,13 +7072,13 @@
     </row>
     <row r="25">
       <c r="A25" s="38" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B25" s="37" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C25" s="35" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D25" s="36"/>
       <c r="E25" s="15"/>
@@ -7094,13 +7099,13 @@
     </row>
     <row r="26">
       <c r="A26" s="33" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B26" s="37" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C26" s="35" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D26" s="36"/>
       <c r="E26" s="15"/>
@@ -7121,13 +7126,13 @@
     </row>
     <row r="27">
       <c r="A27" s="38" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B27" s="37" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C27" s="35" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D27" s="36"/>
       <c r="E27" s="15"/>
@@ -7148,13 +7153,13 @@
     </row>
     <row r="28">
       <c r="A28" s="33" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C28" s="35" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D28" s="36"/>
       <c r="E28" s="15"/>
@@ -7175,13 +7180,13 @@
     </row>
     <row r="29">
       <c r="A29" s="33" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B29" s="39" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C29" s="35" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D29" s="36"/>
       <c r="E29" s="15"/>
@@ -7202,13 +7207,13 @@
     </row>
     <row r="30">
       <c r="A30" s="38" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B30" s="39" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C30" s="35" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D30" s="36"/>
       <c r="E30" s="15"/>
@@ -7219,7 +7224,7 @@
       <c r="J30" s="20"/>
       <c r="K30" s="15"/>
       <c r="M30" s="13" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="N30" s="12">
         <v>0.0</v>
@@ -7232,13 +7237,13 @@
     </row>
     <row r="31">
       <c r="A31" s="13" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
@@ -7249,7 +7254,7 @@
       <c r="J31" s="20"/>
       <c r="K31" s="15"/>
       <c r="M31" s="12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="N31" s="12">
         <v>0.0</v>
@@ -7262,13 +7267,13 @@
     </row>
     <row r="32">
       <c r="A32" s="13" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D32" s="15"/>
       <c r="E32" s="31"/>
@@ -7276,7 +7281,7 @@
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
       <c r="I32" s="12" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="J32" s="20"/>
       <c r="K32" s="15"/>
@@ -7290,13 +7295,13 @@
     </row>
     <row r="33">
       <c r="A33" s="13" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="31" t="b">
@@ -7306,7 +7311,7 @@
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
       <c r="I33" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J33" s="20"/>
       <c r="K33" s="15"/>
@@ -7321,13 +7326,13 @@
     </row>
     <row r="34">
       <c r="A34" s="40" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="41"/>
@@ -7348,13 +7353,13 @@
     </row>
     <row r="35">
       <c r="A35" s="40" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B35" s="42" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D35" s="15"/>
       <c r="E35" s="41"/>
@@ -7375,25 +7380,25 @@
     </row>
     <row r="36">
       <c r="A36" s="43" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D36" s="15"/>
       <c r="E36" s="41" t="b">
         <v>1</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G36" s="15"/>
       <c r="H36" s="15"/>
       <c r="I36" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J36" s="20"/>
       <c r="K36" s="15"/>
@@ -7408,13 +7413,13 @@
     </row>
     <row r="37">
       <c r="A37" s="43" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D37" s="15"/>
       <c r="E37" s="41" t="b">
@@ -7426,7 +7431,7 @@
       <c r="G37" s="15"/>
       <c r="H37" s="15"/>
       <c r="I37" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J37" s="20"/>
       <c r="K37" s="15"/>
@@ -7441,25 +7446,25 @@
     </row>
     <row r="38">
       <c r="A38" s="43" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D38" s="15"/>
       <c r="E38" s="41" t="b">
         <v>1</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G38" s="15"/>
       <c r="H38" s="15"/>
       <c r="I38" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J38" s="20"/>
       <c r="K38" s="15"/>
@@ -7474,13 +7479,13 @@
     </row>
     <row r="39">
       <c r="A39" s="43" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D39" s="15"/>
       <c r="E39" s="41" t="b">
@@ -7492,7 +7497,7 @@
       <c r="G39" s="15"/>
       <c r="H39" s="15"/>
       <c r="I39" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J39" s="20"/>
       <c r="K39" s="15"/>
@@ -7510,10 +7515,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="44" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D40" s="15"/>
       <c r="E40" s="15"/>
@@ -7522,7 +7527,7 @@
       <c r="H40" s="15"/>
       <c r="I40" s="15"/>
       <c r="J40" s="13" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="K40" s="15"/>
       <c r="L40" s="15"/>
@@ -7533,7 +7538,7 @@
       <c r="Q40" s="15"/>
       <c r="R40" s="15"/>
       <c r="S40" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41">
@@ -7541,10 +7546,10 @@
         <v>35</v>
       </c>
       <c r="B41" s="44" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D41" s="15"/>
       <c r="E41" s="15"/>
@@ -7553,7 +7558,7 @@
       <c r="H41" s="15"/>
       <c r="I41" s="15"/>
       <c r="J41" s="13" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="K41" s="15"/>
       <c r="L41" s="15"/>
@@ -7569,10 +7574,10 @@
         <v>31</v>
       </c>
       <c r="B42" s="44" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D42" s="15"/>
       <c r="E42" s="15"/>
@@ -7581,7 +7586,7 @@
       <c r="H42" s="15"/>
       <c r="I42" s="15"/>
       <c r="J42" s="13" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="K42" s="15"/>
       <c r="L42" s="15"/>
@@ -7597,10 +7602,10 @@
         <v>27</v>
       </c>
       <c r="B43" s="44" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D43" s="15"/>
       <c r="E43" s="15"/>
@@ -7609,7 +7614,7 @@
       <c r="H43" s="15"/>
       <c r="I43" s="15"/>
       <c r="J43" s="13" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="K43" s="15"/>
       <c r="L43" s="15"/>
@@ -7622,13 +7627,13 @@
     </row>
     <row r="44">
       <c r="A44" s="13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B44" s="44" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D44" s="15"/>
       <c r="E44" s="15"/>
@@ -7637,7 +7642,7 @@
       <c r="H44" s="15"/>
       <c r="I44" s="15"/>
       <c r="J44" s="13" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="K44" s="15"/>
       <c r="L44" s="15"/>
@@ -7648,18 +7653,18 @@
       <c r="Q44" s="15"/>
       <c r="R44" s="15"/>
       <c r="S44" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="45" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B45" s="46" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C45" s="47" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D45" s="48"/>
       <c r="E45" s="48"/>
@@ -7668,7 +7673,7 @@
       <c r="H45" s="48"/>
       <c r="I45" s="48"/>
       <c r="J45" s="45" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="K45" s="48"/>
       <c r="L45" s="48"/>
@@ -7679,18 +7684,18 @@
       <c r="Q45" s="48"/>
       <c r="R45" s="48"/>
       <c r="S45" s="51" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="45" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B46" s="46" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C46" s="47" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D46" s="48"/>
       <c r="E46" s="48"/>
@@ -7699,7 +7704,7 @@
       <c r="H46" s="48"/>
       <c r="I46" s="48"/>
       <c r="J46" s="45" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="K46" s="48"/>
       <c r="L46" s="48"/>
@@ -7710,18 +7715,18 @@
       <c r="Q46" s="48"/>
       <c r="R46" s="48"/>
       <c r="S46" s="51" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B47" s="44" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D47" s="15"/>
       <c r="E47" s="15"/>
@@ -7730,7 +7735,7 @@
       <c r="H47" s="15"/>
       <c r="I47" s="15"/>
       <c r="J47" s="13" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="K47" s="15"/>
       <c r="L47" s="15"/>
@@ -7741,18 +7746,18 @@
       <c r="Q47" s="15"/>
       <c r="R47" s="15"/>
       <c r="S47" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="13" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B48" s="52" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D48" s="15"/>
       <c r="E48" s="12" t="b">
@@ -7762,7 +7767,7 @@
       <c r="G48" s="15"/>
       <c r="H48" s="15"/>
       <c r="I48" s="12" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J48" s="20"/>
       <c r="L48" s="15"/>
@@ -7776,13 +7781,13 @@
     </row>
     <row r="49">
       <c r="A49" s="13" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B49" s="52" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D49" s="15"/>
       <c r="E49" s="12" t="b">
@@ -7792,7 +7797,7 @@
       <c r="G49" s="15"/>
       <c r="H49" s="15"/>
       <c r="I49" s="12" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J49" s="20"/>
       <c r="L49" s="15"/>
@@ -7806,13 +7811,13 @@
     </row>
     <row r="50">
       <c r="A50" s="13" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B50" s="52" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D50" s="15"/>
       <c r="E50" s="12" t="b">
@@ -7822,7 +7827,7 @@
       <c r="G50" s="15"/>
       <c r="H50" s="15"/>
       <c r="I50" s="12" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J50" s="20"/>
       <c r="L50" s="15"/>
@@ -7836,13 +7841,13 @@
     </row>
     <row r="51">
       <c r="A51" s="13" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B51" s="52" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D51" s="15"/>
       <c r="E51" s="12" t="b">
@@ -7852,7 +7857,7 @@
       <c r="G51" s="15"/>
       <c r="H51" s="15"/>
       <c r="I51" s="12" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J51" s="20"/>
       <c r="L51" s="15"/>
@@ -7866,13 +7871,13 @@
     </row>
     <row r="52">
       <c r="A52" s="13" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B52" s="52" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D52" s="15"/>
       <c r="E52" s="15"/>
@@ -7882,7 +7887,7 @@
       <c r="I52" s="15"/>
       <c r="J52" s="20"/>
       <c r="K52" s="53" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="L52" s="15"/>
       <c r="M52" s="15"/>
@@ -7895,13 +7900,13 @@
     </row>
     <row r="53">
       <c r="A53" s="13" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B53" s="52" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D53" s="15"/>
       <c r="E53" s="12" t="b">
@@ -7911,7 +7916,7 @@
       <c r="G53" s="15"/>
       <c r="H53" s="15"/>
       <c r="I53" s="12" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J53" s="20"/>
       <c r="L53" s="15"/>
@@ -7925,13 +7930,13 @@
     </row>
     <row r="54">
       <c r="A54" s="13" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B54" s="52" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D54" s="15"/>
       <c r="E54" s="15"/>
@@ -7939,7 +7944,7 @@
       <c r="G54" s="15"/>
       <c r="H54" s="15"/>
       <c r="I54" s="12" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J54" s="20"/>
       <c r="L54" s="15"/>
@@ -7953,13 +7958,13 @@
     </row>
     <row r="55">
       <c r="A55" s="13" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B55" s="52" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D55" s="15"/>
       <c r="E55" s="15"/>
@@ -7967,7 +7972,7 @@
       <c r="G55" s="15"/>
       <c r="H55" s="15"/>
       <c r="I55" s="12" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="J55" s="20"/>
       <c r="L55" s="15"/>
@@ -7981,13 +7986,13 @@
     </row>
     <row r="56">
       <c r="A56" s="13" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B56" s="52" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D56" s="15"/>
       <c r="E56" s="15"/>
@@ -7995,7 +8000,7 @@
       <c r="G56" s="15"/>
       <c r="H56" s="15"/>
       <c r="I56" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="J56" s="20"/>
       <c r="L56" s="15"/>
@@ -8009,13 +8014,13 @@
     </row>
     <row r="57">
       <c r="A57" s="13" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B57" s="52" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D57" s="15"/>
       <c r="E57" s="12" t="b">
@@ -8025,7 +8030,7 @@
       <c r="G57" s="15"/>
       <c r="H57" s="15"/>
       <c r="I57" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="J57" s="20"/>
       <c r="L57" s="15"/>
@@ -8039,13 +8044,13 @@
     </row>
     <row r="58">
       <c r="A58" s="13" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B58" s="52" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D58" s="15"/>
       <c r="E58" s="15"/>
@@ -8053,7 +8058,7 @@
       <c r="G58" s="15"/>
       <c r="H58" s="15"/>
       <c r="I58" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="J58" s="20"/>
       <c r="L58" s="15"/>
@@ -8067,13 +8072,13 @@
     </row>
     <row r="59">
       <c r="A59" s="13" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B59" s="52" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D59" s="15"/>
       <c r="E59" s="15"/>
@@ -8081,7 +8086,7 @@
       <c r="G59" s="15"/>
       <c r="H59" s="15"/>
       <c r="I59" s="12" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J59" s="20"/>
       <c r="L59" s="15"/>
@@ -8095,13 +8100,13 @@
     </row>
     <row r="60">
       <c r="A60" s="13" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D60" s="15"/>
       <c r="E60" s="15"/>
@@ -8166,43 +8171,43 @@
         <v>5</v>
       </c>
       <c r="D1" s="54" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E1" s="54" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F1" s="54" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G1" s="54" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H1" s="54" t="s">
         <v>9</v>
       </c>
       <c r="I1" s="54" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="J1" s="57" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="K1" s="54" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="L1" s="58" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="M1" s="56" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="N1" s="54" t="s">
         <v>20</v>
       </c>
       <c r="O1" s="54" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="P1" s="32" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="Q1" s="32"/>
       <c r="R1" s="32"/>
@@ -8210,14 +8215,14 @@
     </row>
     <row r="2">
       <c r="A2" s="13" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C2" s="60"/>
       <c r="D2" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E2" s="43"/>
       <c r="F2" s="12"/>
@@ -8229,7 +8234,7 @@
       <c r="M2" s="15"/>
       <c r="N2" s="15"/>
       <c r="O2" s="12" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="P2" s="31" t="b">
         <v>1</v>
@@ -8240,16 +8245,16 @@
     </row>
     <row r="3">
       <c r="A3" s="18" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B3" s="61" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="12" t="s">
         <v>102</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>101</v>
       </c>
       <c r="E3" s="31"/>
       <c r="F3" s="32"/>
@@ -8262,7 +8267,7 @@
       <c r="M3" s="12"/>
       <c r="N3" s="21"/>
       <c r="O3" s="12" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="P3" s="12" t="b">
         <v>1</v>
@@ -8273,35 +8278,35 @@
     </row>
     <row r="4">
       <c r="A4" s="18" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B4" s="61" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="12"/>
       <c r="E4" s="13" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H4" s="15"/>
       <c r="I4" s="12"/>
       <c r="J4" s="20"/>
       <c r="K4" s="15"/>
       <c r="L4" s="12" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N4" s="21"/>
       <c r="O4" s="12" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="P4" s="12" t="b">
         <v>1</v>
@@ -8312,31 +8317,31 @@
     </row>
     <row r="5">
       <c r="A5" s="18" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B5" s="61" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="12"/>
       <c r="E5" s="13" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="H5" s="15"/>
       <c r="I5" s="12"/>
       <c r="J5" s="20"/>
       <c r="K5" s="15"/>
       <c r="L5" s="12" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N5" s="21"/>
       <c r="O5" s="12"/>
@@ -8347,31 +8352,31 @@
     </row>
     <row r="6">
       <c r="A6" s="18" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B6" s="61" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="12"/>
       <c r="E6" s="13" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="H6" s="15"/>
       <c r="I6" s="12"/>
       <c r="J6" s="20"/>
       <c r="K6" s="15"/>
       <c r="L6" s="12" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N6" s="21"/>
       <c r="O6" s="12"/>
@@ -8382,30 +8387,30 @@
     </row>
     <row r="7">
       <c r="A7" s="18" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B7" s="61" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C7" s="60"/>
       <c r="E7" s="13" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
       <c r="K7" s="61"/>
       <c r="L7" s="13" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N7" s="15"/>
       <c r="O7" s="15"/>
@@ -8416,30 +8421,30 @@
     </row>
     <row r="8">
       <c r="A8" s="18" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B8" s="61" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C8" s="60"/>
       <c r="E8" s="13" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="61"/>
       <c r="L8" s="13" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N8" s="15"/>
       <c r="O8" s="15"/>
@@ -8450,32 +8455,32 @@
     </row>
     <row r="9">
       <c r="A9" s="62" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B9" s="63" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C9" s="64" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D9" s="65"/>
       <c r="E9" s="62" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F9" s="66" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="G9" s="66" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H9" s="67"/>
       <c r="I9" s="68"/>
       <c r="J9" s="68"/>
       <c r="K9" s="69" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L9" s="62" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="M9" s="68"/>
       <c r="N9" s="68"/>
@@ -8487,32 +8492,32 @@
     </row>
     <row r="10">
       <c r="A10" s="62" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B10" s="63" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C10" s="64" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D10" s="65"/>
       <c r="E10" s="62" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F10" s="66" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="G10" s="66" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H10" s="68"/>
       <c r="I10" s="68"/>
       <c r="J10" s="68"/>
       <c r="K10" s="69" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L10" s="62" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="M10" s="68"/>
       <c r="N10" s="68"/>
@@ -8524,32 +8529,32 @@
     </row>
     <row r="11">
       <c r="A11" s="62" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B11" s="63" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C11" s="64" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D11" s="65"/>
       <c r="E11" s="62" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F11" s="66" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G11" s="66" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H11" s="67"/>
       <c r="I11" s="68"/>
       <c r="J11" s="68"/>
       <c r="K11" s="69" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L11" s="62" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="M11" s="68"/>
       <c r="N11" s="68"/>
@@ -8561,32 +8566,32 @@
     </row>
     <row r="12">
       <c r="A12" s="62" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B12" s="63" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C12" s="64" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D12" s="65"/>
       <c r="E12" s="62" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F12" s="66" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G12" s="66" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H12" s="67"/>
       <c r="I12" s="68"/>
       <c r="J12" s="68"/>
       <c r="K12" s="69" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L12" s="62" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="M12" s="68"/>
       <c r="N12" s="68"/>
@@ -8598,20 +8603,20 @@
     </row>
     <row r="13">
       <c r="A13" s="62" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B13" s="63" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C13" s="64" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D13" s="65"/>
       <c r="E13" s="70" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F13" s="66" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G13" s="65"/>
       <c r="H13" s="67"/>
@@ -8633,20 +8638,20 @@
     </row>
     <row r="14">
       <c r="A14" s="62" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B14" s="63" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C14" s="64" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D14" s="65"/>
       <c r="E14" s="70" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F14" s="66" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G14" s="65"/>
       <c r="H14" s="67"/>
@@ -8668,20 +8673,20 @@
     </row>
     <row r="15">
       <c r="A15" s="62" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C15" s="64" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D15" s="65"/>
       <c r="E15" s="70" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F15" s="66" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="G15" s="65"/>
       <c r="H15" s="68"/>
@@ -8703,20 +8708,20 @@
     </row>
     <row r="16">
       <c r="A16" s="62" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C16" s="64" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D16" s="65"/>
       <c r="E16" s="70" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F16" s="66" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="G16" s="65"/>
       <c r="H16" s="67"/>
@@ -8738,32 +8743,32 @@
     </row>
     <row r="17">
       <c r="A17" s="62" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C17" s="64" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D17" s="65"/>
       <c r="E17" s="62" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F17" s="66" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G17" s="66" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="H17" s="67"/>
       <c r="I17" s="68"/>
       <c r="J17" s="68"/>
       <c r="K17" s="69" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L17" s="62" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="M17" s="68"/>
       <c r="N17" s="68"/>
@@ -8775,23 +8780,23 @@
     </row>
     <row r="18">
       <c r="A18" s="71" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B18" s="72" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C18" s="73" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D18" s="74"/>
       <c r="E18" s="75" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F18" s="76" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="G18" s="76" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="H18" s="77"/>
       <c r="I18" s="78"/>
@@ -8800,7 +8805,7 @@
         <v>0.0</v>
       </c>
       <c r="L18" s="79" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M18" s="78"/>
       <c r="N18" s="78"/>
@@ -8812,32 +8817,32 @@
     </row>
     <row r="19">
       <c r="A19" s="80" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B19" s="72" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C19" s="73" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D19" s="74"/>
       <c r="E19" s="71" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F19" s="76" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="G19" s="76" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="H19" s="81"/>
       <c r="I19" s="78"/>
       <c r="J19" s="78"/>
       <c r="K19" s="71" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="L19" s="79" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="M19" s="78"/>
       <c r="N19" s="78"/>
@@ -8849,32 +8854,32 @@
     </row>
     <row r="20">
       <c r="A20" s="80" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B20" s="72" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C20" s="73" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D20" s="74"/>
       <c r="E20" s="71" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F20" s="76" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="G20" s="76" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="H20" s="81"/>
       <c r="I20" s="78"/>
       <c r="J20" s="78"/>
       <c r="K20" s="71" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L20" s="79" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="M20" s="78"/>
       <c r="N20" s="78"/>
@@ -8886,32 +8891,32 @@
     </row>
     <row r="21">
       <c r="A21" s="80" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B21" s="72" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C21" s="73" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D21" s="74"/>
       <c r="E21" s="71" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F21" s="76" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="G21" s="76" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="H21" s="81"/>
       <c r="I21" s="78"/>
       <c r="J21" s="78"/>
       <c r="K21" s="71" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="L21" s="82" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="M21" s="78"/>
       <c r="N21" s="78"/>
@@ -8923,23 +8928,23 @@
     </row>
     <row r="22">
       <c r="A22" s="83" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B22" s="84" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C22" s="85" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D22" s="86"/>
       <c r="E22" s="87" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F22" s="88" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G22" s="88" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="H22" s="89"/>
       <c r="I22" s="90"/>
@@ -8948,7 +8953,7 @@
         <v>0.0</v>
       </c>
       <c r="L22" s="92" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M22" s="90"/>
       <c r="N22" s="90"/>
@@ -8960,32 +8965,32 @@
     </row>
     <row r="23">
       <c r="A23" s="83" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B23" s="84" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C23" s="85" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D23" s="86"/>
       <c r="E23" s="91" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F23" s="93" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="G23" s="93" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H23" s="89"/>
       <c r="I23" s="90"/>
       <c r="J23" s="90"/>
       <c r="K23" s="91" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="L23" s="94" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="M23" s="90"/>
       <c r="N23" s="90"/>
@@ -8997,23 +9002,23 @@
     </row>
     <row r="24">
       <c r="A24" s="95" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B24" s="96" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C24" s="97" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D24" s="98"/>
       <c r="E24" s="99" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F24" s="100" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="G24" s="100" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="H24" s="101"/>
       <c r="I24" s="102"/>
@@ -9022,7 +9027,7 @@
         <v>0.0</v>
       </c>
       <c r="L24" s="104" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M24" s="102"/>
       <c r="N24" s="102"/>
@@ -9034,32 +9039,32 @@
     </row>
     <row r="25">
       <c r="A25" s="95" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B25" s="96" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C25" s="97" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D25" s="98"/>
       <c r="E25" s="103" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F25" s="100" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="G25" s="100" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="H25" s="105"/>
       <c r="I25" s="102"/>
       <c r="J25" s="102"/>
       <c r="K25" s="106" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="L25" s="104" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="M25" s="102"/>
       <c r="N25" s="102"/>
@@ -9071,32 +9076,32 @@
     </row>
     <row r="26">
       <c r="A26" s="107" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B26" s="108" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C26" s="109" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D26" s="110"/>
       <c r="E26" s="111" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F26" s="112" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="G26" s="113" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="H26" s="114"/>
       <c r="I26" s="115"/>
       <c r="J26" s="115"/>
       <c r="K26" s="116" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L26" s="117" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="M26" s="115"/>
       <c r="N26" s="115"/>
@@ -9108,32 +9113,32 @@
     </row>
     <row r="27">
       <c r="A27" s="118" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B27" s="108" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C27" s="109" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D27" s="119"/>
       <c r="E27" s="111" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F27" s="112" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="G27" s="118" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="H27" s="119"/>
       <c r="I27" s="115"/>
       <c r="J27" s="115"/>
       <c r="K27" s="116" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="L27" s="117" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="M27" s="115"/>
       <c r="N27" s="115"/>
@@ -9182,7 +9187,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="122" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E1" s="121" t="s">
         <v>13</v>
@@ -9190,460 +9195,460 @@
     </row>
     <row r="2">
       <c r="A2" s="123" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B2" s="124" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C2" s="124" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D2" s="124"/>
       <c r="E2" s="36"/>
     </row>
     <row r="3">
       <c r="A3" s="123" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B3" s="124" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C3" s="124" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D3" s="124"/>
       <c r="E3" s="36"/>
     </row>
     <row r="4">
       <c r="A4" s="123" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C4" s="124" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D4" s="124"/>
       <c r="E4" s="125" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="123" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C5" s="124" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D5" s="124"/>
       <c r="E5" s="125" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="123" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C6" s="124" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D6" s="124"/>
       <c r="E6" s="126" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="123" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C7" s="124" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D7" s="124"/>
       <c r="E7" s="125" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="123" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B8" s="124" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C8" s="124" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D8" s="124"/>
       <c r="E8" s="36"/>
     </row>
     <row r="9">
       <c r="A9" s="123" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B9" s="124" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C9" s="124" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D9" s="124"/>
       <c r="E9" s="36"/>
     </row>
     <row r="10">
       <c r="A10" s="123" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B10" s="127" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C10" s="124" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D10" s="124"/>
       <c r="E10" s="36"/>
     </row>
     <row r="11">
       <c r="A11" s="123" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B11" s="127" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C11" s="124" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D11" s="124"/>
       <c r="E11" s="36"/>
     </row>
     <row r="12">
       <c r="A12" s="123" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B12" s="127" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C12" s="124" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D12" s="124"/>
       <c r="E12" s="36"/>
     </row>
     <row r="13">
       <c r="A13" s="123" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B13" s="127" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C13" s="124" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D13" s="124"/>
       <c r="E13" s="36"/>
     </row>
     <row r="14">
       <c r="A14" s="123" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B14" s="127" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C14" s="124" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D14" s="124"/>
       <c r="E14" s="36"/>
     </row>
     <row r="15">
       <c r="A15" s="123" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B15" s="127" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C15" s="124" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D15" s="124"/>
       <c r="E15" s="36"/>
     </row>
     <row r="16">
       <c r="A16" s="123" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B16" s="127" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C16" s="124" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D16" s="124"/>
       <c r="E16" s="36"/>
     </row>
     <row r="17">
       <c r="A17" s="123" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B17" s="127" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C17" s="124" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D17" s="124"/>
       <c r="E17" s="36"/>
     </row>
     <row r="18">
       <c r="A18" s="123" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B18" s="124" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C18" s="124" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D18" s="124"/>
       <c r="E18" s="36"/>
     </row>
     <row r="19">
       <c r="A19" s="123" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B19" s="127" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D19" s="128" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E19" s="125" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="123" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C20" s="129" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D20" s="129"/>
       <c r="E20" s="36"/>
     </row>
     <row r="21">
       <c r="A21" s="123" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B21" s="36" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C21" s="129" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D21" s="129"/>
       <c r="E21" s="36"/>
     </row>
     <row r="22">
       <c r="A22" s="123" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D22" s="129" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="E22" s="125" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="123" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B23" s="124" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C23" s="124" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D23" s="124"/>
       <c r="E23" s="125" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="123" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B24" s="124" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C24" s="124" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D24" s="124"/>
       <c r="E24" s="36"/>
     </row>
     <row r="25">
       <c r="A25" s="123" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B25" s="124" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C25" s="124" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D25" s="124"/>
       <c r="E25" s="36"/>
     </row>
     <row r="26">
       <c r="A26" s="123" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B26" s="124" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C26" s="127" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D26" s="127"/>
       <c r="E26" s="127"/>
     </row>
     <row r="27">
       <c r="A27" s="123" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B27" s="124" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C27" s="127" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D27" s="127"/>
       <c r="E27" s="127"/>
     </row>
     <row r="28">
       <c r="A28" s="123" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B28" s="124" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C28" s="127" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D28" s="127"/>
       <c r="E28" s="127"/>
     </row>
     <row r="29">
       <c r="A29" s="123" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B29" s="124" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C29" s="127" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="D29" s="127"/>
       <c r="E29" s="127"/>
     </row>
     <row r="30">
       <c r="A30" s="123" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B30" s="124" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C30" s="127" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D30" s="127"/>
       <c r="E30" s="127"/>
     </row>
     <row r="31">
       <c r="A31" s="123" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B31" s="124" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C31" s="127" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D31" s="127"/>
       <c r="E31" s="127"/>
     </row>
     <row r="32">
       <c r="A32" s="123" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B32" s="124" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C32" s="127" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="D32" s="127"/>
       <c r="E32" s="127"/>
     </row>
     <row r="33">
       <c r="A33" s="123" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B33" s="124" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C33" s="127" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D33" s="127"/>
       <c r="E33" s="127"/>
     </row>
     <row r="34">
       <c r="A34" s="123" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B34" s="124" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C34" s="127" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D34" s="127"/>
       <c r="E34" s="127"/>
     </row>
     <row r="35">
       <c r="A35" s="123" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B35" s="124" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C35" s="127" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="D35" s="127"/>
       <c r="E35" s="127"/>
@@ -9653,10 +9658,10 @@
         <v>54.0</v>
       </c>
       <c r="B36" s="131" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C36" s="36" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D36" s="36"/>
       <c r="E36" s="36"/>
@@ -9666,10 +9671,10 @@
         <v>55.0</v>
       </c>
       <c r="B37" s="131" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C37" s="36" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="D37" s="36"/>
       <c r="E37" s="36"/>
@@ -9679,10 +9684,10 @@
         <v>56.0</v>
       </c>
       <c r="B38" s="131" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C38" s="36" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="D38" s="36"/>
       <c r="E38" s="36"/>
@@ -9692,218 +9697,218 @@
         <v>116.0</v>
       </c>
       <c r="B39" s="131" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C39" s="34" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D39" s="34"/>
       <c r="E39" s="36"/>
     </row>
     <row r="40">
       <c r="A40" s="33" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B40" s="131" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C40" s="34" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D40" s="34"/>
       <c r="E40" s="36"/>
     </row>
     <row r="41">
       <c r="A41" s="33" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B41" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="C41" s="132" t="s">
         <v>110</v>
-      </c>
-      <c r="C41" s="132" t="s">
-        <v>109</v>
       </c>
       <c r="D41" s="132"/>
       <c r="E41" s="36"/>
     </row>
     <row r="42">
       <c r="A42" s="38" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B42" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="C42" s="132" t="s">
         <v>113</v>
-      </c>
-      <c r="C42" s="132" t="s">
-        <v>112</v>
       </c>
       <c r="D42" s="132"/>
       <c r="E42" s="36"/>
     </row>
     <row r="43">
       <c r="A43" s="33" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B43" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="C43" s="132" t="s">
         <v>116</v>
-      </c>
-      <c r="C43" s="132" t="s">
-        <v>115</v>
       </c>
       <c r="D43" s="132"/>
       <c r="E43" s="36"/>
     </row>
     <row r="44">
       <c r="A44" s="38" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B44" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="C44" s="132" t="s">
         <v>119</v>
-      </c>
-      <c r="C44" s="132" t="s">
-        <v>118</v>
       </c>
       <c r="D44" s="132"/>
       <c r="E44" s="36"/>
     </row>
     <row r="45">
       <c r="A45" s="33" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B45" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="C45" s="132" t="s">
         <v>122</v>
-      </c>
-      <c r="C45" s="132" t="s">
-        <v>121</v>
       </c>
       <c r="D45" s="132"/>
       <c r="E45" s="36"/>
     </row>
     <row r="46">
       <c r="A46" s="38" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B46" s="35" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C46" s="132" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D46" s="132"/>
       <c r="E46" s="36"/>
     </row>
     <row r="47">
       <c r="A47" s="33" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B47" s="35" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C47" s="132" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="D47" s="132"/>
       <c r="E47" s="36"/>
     </row>
     <row r="48">
       <c r="A48" s="38" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B48" s="35" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C48" s="132" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="D48" s="132"/>
       <c r="E48" s="36"/>
     </row>
     <row r="49">
       <c r="A49" s="33" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B49" s="35" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C49" s="132" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D49" s="132"/>
       <c r="E49" s="36"/>
     </row>
     <row r="50">
       <c r="A50" s="33" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B50" s="35" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C50" s="132" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D50" s="132"/>
       <c r="E50" s="36"/>
     </row>
     <row r="51">
       <c r="A51" s="33" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B51" s="35" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C51" s="132" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="D51" s="132"/>
       <c r="E51" s="36"/>
     </row>
     <row r="52">
       <c r="A52" s="33" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B52" s="35" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C52" s="133" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="D52" s="134"/>
       <c r="E52" s="36"/>
     </row>
     <row r="53">
       <c r="A53" s="33" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B53" s="35" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C53" s="133" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="D53" s="135"/>
       <c r="E53" s="36"/>
     </row>
     <row r="54">
       <c r="A54" s="33" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B54" s="35" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C54" s="133" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="D54" s="135"/>
       <c r="E54" s="36"/>
     </row>
     <row r="55">
       <c r="A55" s="38" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C55" s="52" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="D55" s="52"/>
       <c r="E55" s="36"/>
@@ -9939,33 +9944,33 @@
         <v>1</v>
       </c>
       <c r="C1" s="54" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="D1" s="54" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="E1" s="54" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="F1" s="54" t="s">
         <v>9</v>
       </c>
       <c r="G1" s="56" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="13" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>39</v>
@@ -9975,16 +9980,16 @@
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>35</v>
@@ -9994,16 +9999,16 @@
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>31</v>
@@ -10013,16 +10018,16 @@
     </row>
     <row r="5">
       <c r="A5" s="13" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>27</v>
@@ -10032,95 +10037,95 @@
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F6" s="136"/>
       <c r="G6" s="15"/>
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F7" s="136"/>
       <c r="G7" s="15"/>
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F8" s="136"/>
       <c r="G8" s="15"/>
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F9" s="136"/>
       <c r="G9" s="15"/>
     </row>
     <row r="10">
       <c r="A10" s="13" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F10" s="136"/>
       <c r="G10" s="15"/>
@@ -10154,31 +10159,31 @@
         <v>5</v>
       </c>
       <c r="D1" s="54" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D2" s="15"/>
       <c r="F2" s="2" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D3" s="15"/>
       <c r="F3" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
   </sheetData>
@@ -10220,19 +10225,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="137" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D1" s="137" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="G1" s="137" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>20</v>
@@ -10241,71 +10246,71 @@
         <v>5</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="K1" s="138" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="C2" s="139"/>
       <c r="D2" s="13"/>
       <c r="G2" s="140"/>
       <c r="I2" s="2" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="C3" s="140"/>
       <c r="D3" s="13"/>
       <c r="G3" s="140"/>
       <c r="I3" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="4" ht="20.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C4" s="140"/>
       <c r="D4" s="13"/>
       <c r="E4" s="141"/>
       <c r="G4" s="142"/>
       <c r="I4" s="2" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="J4" s="143"/>
       <c r="K4" s="2" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="C5" s="140"/>
       <c r="D5" s="13"/>
@@ -10313,39 +10318,39 @@
       <c r="F5" s="142"/>
       <c r="G5" s="142"/>
       <c r="I5" s="2" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="J5" s="143"/>
       <c r="K5" s="2" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="6" ht="22.5" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="144"/>
       <c r="G6" s="140"/>
       <c r="I6" s="2" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="7" ht="22.5" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="144"/>
@@ -10353,13 +10358,13 @@
     </row>
     <row r="8" ht="22.5" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="144"/>
@@ -10387,16 +10392,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="32" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
@@ -10412,13 +10417,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
@@ -10459,13 +10464,13 @@
     </row>
     <row r="5">
       <c r="A5" s="15" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -10482,10 +10487,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -10500,10 +10505,10 @@
     <row r="7">
       <c r="A7" s="15"/>
       <c r="B7" s="15" t="s">
+        <v>549</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>548</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>547</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -10518,10 +10523,10 @@
     <row r="8">
       <c r="A8" s="15"/>
       <c r="B8" s="15" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -10536,10 +10541,10 @@
     <row r="9">
       <c r="A9" s="15"/>
       <c r="B9" s="15" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -10567,7 +10572,7 @@
     </row>
     <row r="11">
       <c r="A11" s="15" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="B11" s="145" t="s">
         <v>4</v>
@@ -10585,7 +10590,7 @@
     </row>
     <row r="12">
       <c r="A12" s="15" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B12" s="146" t="s">
         <v>3</v>
@@ -10603,10 +10608,10 @@
     </row>
     <row r="13">
       <c r="A13" s="15" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="B13" s="146" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="L13" s="15"/>
     </row>
@@ -10636,38 +10641,38 @@
     </row>
     <row r="20">
       <c r="A20" s="147" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B20" s="148" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="L20" s="15"/>
     </row>
     <row r="21">
       <c r="A21" s="147" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B21" s="148" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="L21" s="15"/>
     </row>
     <row r="22">
       <c r="A22" s="147" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="B22" s="149"/>
       <c r="L22" s="15"/>
     </row>
     <row r="23" hidden="1">
       <c r="A23" s="15" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="L23" s="15"/>
     </row>
     <row r="24" hidden="1">
       <c r="A24" s="15" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="L24" s="15"/>
     </row>
@@ -10724,42 +10729,42 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="151" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="C2" s="152" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="153" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="C3" s="152" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="154" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="C4" s="152" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="154" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="C5" s="152" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aacar updates for v2 changes, splen fix layer order for neuron 1
</commit_message>
<xml_diff>
--- a/models/spleen/source/spleen.xlsx
+++ b/models/spleen/source/spleen.xlsx
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="627">
   <si>
     <t>id</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>ApiNATOMY model of the spleen</t>
+  </si>
+  <si>
+    <t>splen</t>
   </si>
   <si>
     <t>ontologyTerms</t>
@@ -842,6 +845,9 @@
   </si>
   <si>
     <t>ns_seg_out</t>
+  </si>
+  <si>
+    <t>2,0</t>
   </si>
   <si>
     <t>T8,n-gspl</t>
@@ -2954,7 +2960,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2985,63 +2991,63 @@
         <v>1</v>
       </c>
       <c r="C1" s="156" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="155" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E1" s="155" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F1" s="155" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="2" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="39" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
   </sheetData>
@@ -3065,106 +3071,106 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="157" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="B2" s="158" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="157" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="B3" s="159" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="157" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="B4" s="160" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="157" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="B5" s="160" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="157" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="B6" s="160" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="157" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="B7" s="160" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="157" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="B8" s="160" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="157" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="B9" s="160" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="157" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="B10" s="160" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="157" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="B11" s="160" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="B12" s="152" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="B13" s="161" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
     </row>
   </sheetData>
@@ -3202,103 +3208,103 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="162" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="163" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="163" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>611</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="163" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="163" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="B5" s="164" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="163" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="B6" s="164" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="163" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="B7" s="164" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="165"/>
       <c r="B8" s="164" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="165"/>
       <c r="B9" s="164" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="165"/>
       <c r="B10" s="164" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="165"/>
       <c r="B11" s="164" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="165"/>
       <c r="B12" s="164" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
     </row>
     <row r="13">
@@ -6311,85 +6317,85 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P1" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Q1" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
       <c r="I2" s="12"/>
       <c r="J2" s="13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
       <c r="M2" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N2" s="16"/>
       <c r="O2" s="15"/>
@@ -6400,29 +6406,29 @@
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
       <c r="F3" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
       <c r="I3" s="12"/>
       <c r="J3" s="13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>
       <c r="M3" s="12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N3" s="16"/>
       <c r="O3" s="15"/>
@@ -6433,29 +6439,29 @@
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
       <c r="F4" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
       <c r="I4" s="12"/>
       <c r="J4" s="13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
       <c r="M4" s="12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N4" s="16"/>
       <c r="O4" s="15"/>
@@ -6466,29 +6472,29 @@
     </row>
     <row r="5">
       <c r="A5" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
       <c r="F5" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
       <c r="I5" s="12"/>
       <c r="J5" s="13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
       <c r="M5" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N5" s="16"/>
       <c r="O5" s="15"/>
@@ -6499,13 +6505,13 @@
     </row>
     <row r="6" ht="46.5" customHeight="1">
       <c r="A6" s="13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="19" t="b">
@@ -6515,7 +6521,7 @@
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
       <c r="I6" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J6" s="20"/>
       <c r="K6" s="15"/>
@@ -6530,32 +6536,32 @@
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
       <c r="F7" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
       <c r="I7" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J7" s="20"/>
       <c r="K7" s="15"/>
       <c r="L7" s="15"/>
       <c r="M7" s="21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N7" s="21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="O7" s="15"/>
       <c r="P7" s="15"/>
@@ -6565,13 +6571,13 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -6583,7 +6589,7 @@
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
       <c r="M8" s="13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N8" s="16"/>
       <c r="O8" s="15"/>
@@ -6594,13 +6600,13 @@
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -6612,7 +6618,7 @@
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
       <c r="M9" s="13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="N9" s="16"/>
       <c r="O9" s="15"/>
@@ -6623,13 +6629,13 @@
     </row>
     <row r="10">
       <c r="A10" s="13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -6641,7 +6647,7 @@
       <c r="K10" s="15"/>
       <c r="L10" s="15"/>
       <c r="M10" s="21" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="N10" s="21"/>
       <c r="O10" s="15"/>
@@ -6652,13 +6658,13 @@
     </row>
     <row r="11">
       <c r="A11" s="13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
@@ -6670,7 +6676,7 @@
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
       <c r="M11" s="12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N11" s="16"/>
       <c r="O11" s="15"/>
@@ -6681,13 +6687,13 @@
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
@@ -6699,7 +6705,7 @@
       <c r="K12" s="15"/>
       <c r="L12" s="15"/>
       <c r="M12" s="13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N12" s="16"/>
       <c r="O12" s="15"/>
@@ -6710,23 +6716,23 @@
     </row>
     <row r="13">
       <c r="A13" s="13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
       <c r="I13" s="22" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J13" s="20"/>
       <c r="K13" s="15"/>
@@ -6740,18 +6746,18 @@
     </row>
     <row r="14">
       <c r="A14" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
       <c r="F14" s="23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
@@ -6759,10 +6765,10 @@
       <c r="K14" s="15"/>
       <c r="L14" s="15"/>
       <c r="M14" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N14" s="21" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="O14" s="15"/>
       <c r="P14" s="15"/>
@@ -6772,18 +6778,18 @@
     </row>
     <row r="15">
       <c r="A15" s="13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
@@ -6792,10 +6798,10 @@
       <c r="K15" s="15"/>
       <c r="L15" s="15"/>
       <c r="M15" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N15" s="21" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="O15" s="15"/>
       <c r="P15" s="15"/>
@@ -6805,18 +6811,18 @@
     </row>
     <row r="16">
       <c r="A16" s="24" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D16" s="26"/>
       <c r="E16" s="26"/>
       <c r="F16" s="27" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G16" s="26"/>
       <c r="H16" s="26"/>
@@ -6825,10 +6831,10 @@
       <c r="K16" s="26"/>
       <c r="L16" s="26"/>
       <c r="M16" s="29" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N16" s="30" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="O16" s="26"/>
       <c r="P16" s="26"/>
@@ -6838,13 +6844,13 @@
     </row>
     <row r="17">
       <c r="A17" s="13" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
@@ -6856,7 +6862,7 @@
       <c r="K17" s="15"/>
       <c r="L17" s="15"/>
       <c r="M17" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N17" s="21"/>
       <c r="O17" s="15"/>
@@ -6867,18 +6873,18 @@
     </row>
     <row r="18">
       <c r="A18" s="13" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
       <c r="F18" s="23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
@@ -6887,10 +6893,10 @@
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
       <c r="M18" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N18" s="21" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="O18" s="15"/>
       <c r="P18" s="15"/>
@@ -6900,13 +6906,13 @@
     </row>
     <row r="19">
       <c r="A19" s="13" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
@@ -6918,7 +6924,7 @@
       <c r="K19" s="15"/>
       <c r="L19" s="15"/>
       <c r="M19" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N19" s="21"/>
       <c r="O19" s="15"/>
@@ -6929,18 +6935,18 @@
     </row>
     <row r="20">
       <c r="A20" s="13" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="13" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
@@ -6949,10 +6955,10 @@
       <c r="K20" s="15"/>
       <c r="L20" s="15"/>
       <c r="M20" s="12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="N20" s="21" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="O20" s="15"/>
       <c r="P20" s="15"/>
@@ -6962,13 +6968,13 @@
     </row>
     <row r="21">
       <c r="A21" s="13" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="31"/>
@@ -6989,13 +6995,13 @@
     </row>
     <row r="22">
       <c r="A22" s="18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="31"/>
@@ -7003,7 +7009,7 @@
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
       <c r="I22" s="12" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J22" s="20"/>
       <c r="K22" s="15"/>
@@ -7018,13 +7024,13 @@
     </row>
     <row r="23">
       <c r="A23" s="33" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C23" s="35" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D23" s="36"/>
       <c r="E23" s="15"/>
@@ -7045,13 +7051,13 @@
     </row>
     <row r="24">
       <c r="A24" s="33" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B24" s="37" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C24" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D24" s="36"/>
       <c r="E24" s="15"/>
@@ -7072,13 +7078,13 @@
     </row>
     <row r="25">
       <c r="A25" s="38" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B25" s="37" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C25" s="35" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D25" s="36"/>
       <c r="E25" s="15"/>
@@ -7099,13 +7105,13 @@
     </row>
     <row r="26">
       <c r="A26" s="33" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B26" s="37" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C26" s="35" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D26" s="36"/>
       <c r="E26" s="15"/>
@@ -7126,13 +7132,13 @@
     </row>
     <row r="27">
       <c r="A27" s="38" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B27" s="37" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C27" s="35" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D27" s="36"/>
       <c r="E27" s="15"/>
@@ -7153,13 +7159,13 @@
     </row>
     <row r="28">
       <c r="A28" s="33" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C28" s="35" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D28" s="36"/>
       <c r="E28" s="15"/>
@@ -7180,13 +7186,13 @@
     </row>
     <row r="29">
       <c r="A29" s="33" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B29" s="39" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C29" s="35" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D29" s="36"/>
       <c r="E29" s="15"/>
@@ -7207,13 +7213,13 @@
     </row>
     <row r="30">
       <c r="A30" s="38" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B30" s="39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C30" s="35" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D30" s="36"/>
       <c r="E30" s="15"/>
@@ -7224,7 +7230,7 @@
       <c r="J30" s="20"/>
       <c r="K30" s="15"/>
       <c r="M30" s="13" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="N30" s="12">
         <v>0.0</v>
@@ -7237,13 +7243,13 @@
     </row>
     <row r="31">
       <c r="A31" s="13" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
@@ -7254,7 +7260,7 @@
       <c r="J31" s="20"/>
       <c r="K31" s="15"/>
       <c r="M31" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="N31" s="12">
         <v>0.0</v>
@@ -7267,13 +7273,13 @@
     </row>
     <row r="32">
       <c r="A32" s="13" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D32" s="15"/>
       <c r="E32" s="31"/>
@@ -7281,7 +7287,7 @@
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
       <c r="I32" s="12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J32" s="20"/>
       <c r="K32" s="15"/>
@@ -7295,13 +7301,13 @@
     </row>
     <row r="33">
       <c r="A33" s="13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="31" t="b">
@@ -7311,7 +7317,7 @@
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
       <c r="I33" s="15" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J33" s="20"/>
       <c r="K33" s="15"/>
@@ -7326,13 +7332,13 @@
     </row>
     <row r="34">
       <c r="A34" s="40" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="41"/>
@@ -7353,13 +7359,13 @@
     </row>
     <row r="35">
       <c r="A35" s="40" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B35" s="42" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D35" s="15"/>
       <c r="E35" s="41"/>
@@ -7380,25 +7386,25 @@
     </row>
     <row r="36">
       <c r="A36" s="43" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D36" s="15"/>
       <c r="E36" s="41" t="b">
         <v>1</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G36" s="15"/>
       <c r="H36" s="15"/>
       <c r="I36" s="15" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J36" s="20"/>
       <c r="K36" s="15"/>
@@ -7413,25 +7419,25 @@
     </row>
     <row r="37">
       <c r="A37" s="43" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D37" s="15"/>
       <c r="E37" s="41" t="b">
         <v>1</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G37" s="15"/>
       <c r="H37" s="15"/>
       <c r="I37" s="15" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J37" s="20"/>
       <c r="K37" s="15"/>
@@ -7446,25 +7452,25 @@
     </row>
     <row r="38">
       <c r="A38" s="43" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D38" s="15"/>
       <c r="E38" s="41" t="b">
         <v>1</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G38" s="15"/>
       <c r="H38" s="15"/>
       <c r="I38" s="15" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J38" s="20"/>
       <c r="K38" s="15"/>
@@ -7479,25 +7485,25 @@
     </row>
     <row r="39">
       <c r="A39" s="43" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D39" s="15"/>
       <c r="E39" s="41" t="b">
         <v>1</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G39" s="15"/>
       <c r="H39" s="15"/>
       <c r="I39" s="15" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J39" s="20"/>
       <c r="K39" s="15"/>
@@ -7512,13 +7518,13 @@
     </row>
     <row r="40">
       <c r="A40" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B40" s="44" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D40" s="15"/>
       <c r="E40" s="15"/>
@@ -7527,7 +7533,7 @@
       <c r="H40" s="15"/>
       <c r="I40" s="15"/>
       <c r="J40" s="13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K40" s="15"/>
       <c r="L40" s="15"/>
@@ -7538,18 +7544,18 @@
       <c r="Q40" s="15"/>
       <c r="R40" s="15"/>
       <c r="S40" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B41" s="44" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D41" s="15"/>
       <c r="E41" s="15"/>
@@ -7558,7 +7564,7 @@
       <c r="H41" s="15"/>
       <c r="I41" s="15"/>
       <c r="J41" s="13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K41" s="15"/>
       <c r="L41" s="15"/>
@@ -7571,13 +7577,13 @@
     </row>
     <row r="42">
       <c r="A42" s="13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B42" s="44" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D42" s="15"/>
       <c r="E42" s="15"/>
@@ -7586,7 +7592,7 @@
       <c r="H42" s="15"/>
       <c r="I42" s="15"/>
       <c r="J42" s="13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K42" s="15"/>
       <c r="L42" s="15"/>
@@ -7599,13 +7605,13 @@
     </row>
     <row r="43">
       <c r="A43" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B43" s="44" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D43" s="15"/>
       <c r="E43" s="15"/>
@@ -7614,7 +7620,7 @@
       <c r="H43" s="15"/>
       <c r="I43" s="15"/>
       <c r="J43" s="13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K43" s="15"/>
       <c r="L43" s="15"/>
@@ -7627,13 +7633,13 @@
     </row>
     <row r="44">
       <c r="A44" s="13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B44" s="44" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D44" s="15"/>
       <c r="E44" s="15"/>
@@ -7642,7 +7648,7 @@
       <c r="H44" s="15"/>
       <c r="I44" s="15"/>
       <c r="J44" s="13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K44" s="15"/>
       <c r="L44" s="15"/>
@@ -7653,18 +7659,18 @@
       <c r="Q44" s="15"/>
       <c r="R44" s="15"/>
       <c r="S44" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="45" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B45" s="46" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C45" s="47" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D45" s="48"/>
       <c r="E45" s="48"/>
@@ -7673,7 +7679,7 @@
       <c r="H45" s="48"/>
       <c r="I45" s="48"/>
       <c r="J45" s="45" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K45" s="48"/>
       <c r="L45" s="48"/>
@@ -7684,18 +7690,18 @@
       <c r="Q45" s="48"/>
       <c r="R45" s="48"/>
       <c r="S45" s="51" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="45" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B46" s="46" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C46" s="47" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D46" s="48"/>
       <c r="E46" s="48"/>
@@ -7704,7 +7710,7 @@
       <c r="H46" s="48"/>
       <c r="I46" s="48"/>
       <c r="J46" s="45" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K46" s="48"/>
       <c r="L46" s="48"/>
@@ -7715,18 +7721,18 @@
       <c r="Q46" s="48"/>
       <c r="R46" s="48"/>
       <c r="S46" s="51" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B47" s="44" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D47" s="15"/>
       <c r="E47" s="15"/>
@@ -7735,7 +7741,7 @@
       <c r="H47" s="15"/>
       <c r="I47" s="15"/>
       <c r="J47" s="13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K47" s="15"/>
       <c r="L47" s="15"/>
@@ -7746,18 +7752,18 @@
       <c r="Q47" s="15"/>
       <c r="R47" s="15"/>
       <c r="S47" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="13" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B48" s="52" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D48" s="15"/>
       <c r="E48" s="12" t="b">
@@ -7767,7 +7773,7 @@
       <c r="G48" s="15"/>
       <c r="H48" s="15"/>
       <c r="I48" s="12" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J48" s="20"/>
       <c r="L48" s="15"/>
@@ -7781,13 +7787,13 @@
     </row>
     <row r="49">
       <c r="A49" s="13" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B49" s="52" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D49" s="15"/>
       <c r="E49" s="12" t="b">
@@ -7797,7 +7803,7 @@
       <c r="G49" s="15"/>
       <c r="H49" s="15"/>
       <c r="I49" s="12" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J49" s="20"/>
       <c r="L49" s="15"/>
@@ -7811,13 +7817,13 @@
     </row>
     <row r="50">
       <c r="A50" s="13" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B50" s="52" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D50" s="15"/>
       <c r="E50" s="12" t="b">
@@ -7827,7 +7833,7 @@
       <c r="G50" s="15"/>
       <c r="H50" s="15"/>
       <c r="I50" s="12" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J50" s="20"/>
       <c r="L50" s="15"/>
@@ -7841,13 +7847,13 @@
     </row>
     <row r="51">
       <c r="A51" s="13" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B51" s="52" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D51" s="15"/>
       <c r="E51" s="12" t="b">
@@ -7857,7 +7863,7 @@
       <c r="G51" s="15"/>
       <c r="H51" s="15"/>
       <c r="I51" s="12" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J51" s="20"/>
       <c r="L51" s="15"/>
@@ -7871,13 +7877,13 @@
     </row>
     <row r="52">
       <c r="A52" s="13" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B52" s="52" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D52" s="15"/>
       <c r="E52" s="15"/>
@@ -7887,7 +7893,7 @@
       <c r="I52" s="15"/>
       <c r="J52" s="20"/>
       <c r="K52" s="53" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="L52" s="15"/>
       <c r="M52" s="15"/>
@@ -7900,13 +7906,13 @@
     </row>
     <row r="53">
       <c r="A53" s="13" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B53" s="52" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D53" s="15"/>
       <c r="E53" s="12" t="b">
@@ -7916,7 +7922,7 @@
       <c r="G53" s="15"/>
       <c r="H53" s="15"/>
       <c r="I53" s="12" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J53" s="20"/>
       <c r="L53" s="15"/>
@@ -7930,13 +7936,13 @@
     </row>
     <row r="54">
       <c r="A54" s="13" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B54" s="52" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D54" s="15"/>
       <c r="E54" s="15"/>
@@ -7944,7 +7950,7 @@
       <c r="G54" s="15"/>
       <c r="H54" s="15"/>
       <c r="I54" s="12" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J54" s="20"/>
       <c r="L54" s="15"/>
@@ -7958,13 +7964,13 @@
     </row>
     <row r="55">
       <c r="A55" s="13" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B55" s="52" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D55" s="15"/>
       <c r="E55" s="15"/>
@@ -7972,7 +7978,7 @@
       <c r="G55" s="15"/>
       <c r="H55" s="15"/>
       <c r="I55" s="12" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="J55" s="20"/>
       <c r="L55" s="15"/>
@@ -7986,13 +7992,13 @@
     </row>
     <row r="56">
       <c r="A56" s="13" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B56" s="52" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D56" s="15"/>
       <c r="E56" s="15"/>
@@ -8000,7 +8006,7 @@
       <c r="G56" s="15"/>
       <c r="H56" s="15"/>
       <c r="I56" s="12" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="J56" s="20"/>
       <c r="L56" s="15"/>
@@ -8014,13 +8020,13 @@
     </row>
     <row r="57">
       <c r="A57" s="13" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B57" s="52" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D57" s="15"/>
       <c r="E57" s="12" t="b">
@@ -8030,7 +8036,7 @@
       <c r="G57" s="15"/>
       <c r="H57" s="15"/>
       <c r="I57" s="12" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="J57" s="20"/>
       <c r="L57" s="15"/>
@@ -8044,13 +8050,13 @@
     </row>
     <row r="58">
       <c r="A58" s="13" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B58" s="52" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D58" s="15"/>
       <c r="E58" s="15"/>
@@ -8058,7 +8064,7 @@
       <c r="G58" s="15"/>
       <c r="H58" s="15"/>
       <c r="I58" s="12" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="J58" s="20"/>
       <c r="L58" s="15"/>
@@ -8072,13 +8078,13 @@
     </row>
     <row r="59">
       <c r="A59" s="13" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B59" s="52" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D59" s="15"/>
       <c r="E59" s="15"/>
@@ -8086,7 +8092,7 @@
       <c r="G59" s="15"/>
       <c r="H59" s="15"/>
       <c r="I59" s="12" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J59" s="20"/>
       <c r="L59" s="15"/>
@@ -8100,13 +8106,13 @@
     </row>
     <row r="60">
       <c r="A60" s="13" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D60" s="15"/>
       <c r="E60" s="15"/>
@@ -8168,46 +8174,46 @@
         <v>1</v>
       </c>
       <c r="C1" s="56" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="54" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E1" s="54" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F1" s="54" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G1" s="54" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H1" s="54" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I1" s="54" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="J1" s="57" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="K1" s="54" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L1" s="58" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="M1" s="56" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="N1" s="54" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O1" s="54" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="P1" s="32" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="Q1" s="32"/>
       <c r="R1" s="32"/>
@@ -8215,14 +8221,14 @@
     </row>
     <row r="2">
       <c r="A2" s="13" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C2" s="60"/>
       <c r="D2" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E2" s="43"/>
       <c r="F2" s="12"/>
@@ -8234,7 +8240,7 @@
       <c r="M2" s="15"/>
       <c r="N2" s="15"/>
       <c r="O2" s="12" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="P2" s="31" t="b">
         <v>1</v>
@@ -8245,16 +8251,16 @@
     </row>
     <row r="3">
       <c r="A3" s="18" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B3" s="61" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="12" t="s">
         <v>103</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>102</v>
       </c>
       <c r="E3" s="31"/>
       <c r="F3" s="32"/>
@@ -8267,7 +8273,7 @@
       <c r="M3" s="12"/>
       <c r="N3" s="21"/>
       <c r="O3" s="12" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="P3" s="12" t="b">
         <v>1</v>
@@ -8278,35 +8284,35 @@
     </row>
     <row r="4">
       <c r="A4" s="18" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B4" s="61" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="12"/>
       <c r="E4" s="13" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H4" s="15"/>
       <c r="I4" s="12"/>
       <c r="J4" s="20"/>
       <c r="K4" s="15"/>
       <c r="L4" s="12" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="N4" s="21"/>
       <c r="O4" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="P4" s="12" t="b">
         <v>1</v>
@@ -8317,31 +8323,31 @@
     </row>
     <row r="5">
       <c r="A5" s="18" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B5" s="61" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="12"/>
       <c r="E5" s="13" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="H5" s="15"/>
       <c r="I5" s="12"/>
       <c r="J5" s="20"/>
       <c r="K5" s="15"/>
       <c r="L5" s="12" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N5" s="21"/>
       <c r="O5" s="12"/>
@@ -8352,31 +8358,31 @@
     </row>
     <row r="6">
       <c r="A6" s="18" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B6" s="61" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="12"/>
       <c r="E6" s="13" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="H6" s="15"/>
       <c r="I6" s="12"/>
       <c r="J6" s="20"/>
       <c r="K6" s="15"/>
       <c r="L6" s="12" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N6" s="21"/>
       <c r="O6" s="12"/>
@@ -8387,30 +8393,30 @@
     </row>
     <row r="7">
       <c r="A7" s="18" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B7" s="61" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C7" s="60"/>
       <c r="E7" s="13" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
       <c r="K7" s="61"/>
       <c r="L7" s="13" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="N7" s="15"/>
       <c r="O7" s="15"/>
@@ -8421,30 +8427,30 @@
     </row>
     <row r="8">
       <c r="A8" s="18" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B8" s="61" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C8" s="60"/>
       <c r="E8" s="13" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="61"/>
       <c r="L8" s="13" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N8" s="15"/>
       <c r="O8" s="15"/>
@@ -8455,32 +8461,32 @@
     </row>
     <row r="9">
       <c r="A9" s="62" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B9" s="63" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C9" s="64" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D9" s="65"/>
       <c r="E9" s="62" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F9" s="66" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G9" s="66" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H9" s="67"/>
       <c r="I9" s="68"/>
       <c r="J9" s="68"/>
       <c r="K9" s="69" t="s">
-        <v>76</v>
+        <v>259</v>
       </c>
       <c r="L9" s="62" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="M9" s="68"/>
       <c r="N9" s="68"/>
@@ -8492,32 +8498,32 @@
     </row>
     <row r="10">
       <c r="A10" s="62" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B10" s="63" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C10" s="64" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D10" s="65"/>
       <c r="E10" s="62" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F10" s="66" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="G10" s="66" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H10" s="68"/>
       <c r="I10" s="68"/>
       <c r="J10" s="68"/>
       <c r="K10" s="69" t="s">
-        <v>76</v>
+        <v>259</v>
       </c>
       <c r="L10" s="62" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="M10" s="68"/>
       <c r="N10" s="68"/>
@@ -8529,32 +8535,32 @@
     </row>
     <row r="11">
       <c r="A11" s="62" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B11" s="63" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C11" s="64" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D11" s="65"/>
       <c r="E11" s="62" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F11" s="66" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="G11" s="66" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H11" s="67"/>
       <c r="I11" s="68"/>
       <c r="J11" s="68"/>
       <c r="K11" s="69" t="s">
-        <v>76</v>
+        <v>259</v>
       </c>
       <c r="L11" s="62" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="M11" s="68"/>
       <c r="N11" s="68"/>
@@ -8566,32 +8572,32 @@
     </row>
     <row r="12">
       <c r="A12" s="62" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B12" s="63" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C12" s="64" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D12" s="65"/>
       <c r="E12" s="62" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F12" s="66" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="G12" s="66" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H12" s="67"/>
       <c r="I12" s="68"/>
       <c r="J12" s="68"/>
       <c r="K12" s="69" t="s">
-        <v>76</v>
+        <v>259</v>
       </c>
       <c r="L12" s="62" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="M12" s="68"/>
       <c r="N12" s="68"/>
@@ -8603,30 +8609,30 @@
     </row>
     <row r="13">
       <c r="A13" s="62" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B13" s="63" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C13" s="64" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D13" s="65"/>
       <c r="E13" s="70" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F13" s="66" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="G13" s="65"/>
       <c r="H13" s="67"/>
       <c r="I13" s="68"/>
       <c r="J13" s="68"/>
       <c r="K13" s="69">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="L13" s="62" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M13" s="68"/>
       <c r="N13" s="68"/>
@@ -8638,30 +8644,30 @@
     </row>
     <row r="14">
       <c r="A14" s="62" t="s">
+        <v>277</v>
+      </c>
+      <c r="B14" s="63" t="s">
+        <v>278</v>
+      </c>
+      <c r="C14" s="64" t="s">
         <v>275</v>
-      </c>
-      <c r="B14" s="63" t="s">
-        <v>276</v>
-      </c>
-      <c r="C14" s="64" t="s">
-        <v>273</v>
       </c>
       <c r="D14" s="65"/>
       <c r="E14" s="70" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F14" s="66" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="G14" s="65"/>
       <c r="H14" s="67"/>
       <c r="I14" s="68"/>
       <c r="J14" s="68"/>
       <c r="K14" s="69">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="L14" s="62" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M14" s="68"/>
       <c r="N14" s="68"/>
@@ -8673,30 +8679,30 @@
     </row>
     <row r="15">
       <c r="A15" s="62" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C15" s="64" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D15" s="65"/>
       <c r="E15" s="70" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F15" s="66" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="G15" s="65"/>
       <c r="H15" s="68"/>
       <c r="I15" s="68"/>
       <c r="J15" s="68"/>
       <c r="K15" s="69">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="L15" s="62" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M15" s="68"/>
       <c r="N15" s="68"/>
@@ -8708,30 +8714,30 @@
     </row>
     <row r="16">
       <c r="A16" s="62" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C16" s="64" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D16" s="65"/>
       <c r="E16" s="70" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F16" s="66" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="G16" s="65"/>
       <c r="H16" s="67"/>
       <c r="I16" s="68"/>
       <c r="J16" s="68"/>
       <c r="K16" s="69">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="L16" s="62" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M16" s="68"/>
       <c r="N16" s="68"/>
@@ -8743,32 +8749,32 @@
     </row>
     <row r="17">
       <c r="A17" s="62" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C17" s="64" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D17" s="65"/>
       <c r="E17" s="62" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F17" s="66" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G17" s="66" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="H17" s="67"/>
       <c r="I17" s="68"/>
       <c r="J17" s="68"/>
       <c r="K17" s="69" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L17" s="62" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="M17" s="68"/>
       <c r="N17" s="68"/>
@@ -8780,23 +8786,23 @@
     </row>
     <row r="18">
       <c r="A18" s="71" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B18" s="72" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C18" s="73" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D18" s="74"/>
       <c r="E18" s="75" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F18" s="76" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="G18" s="76" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="H18" s="77"/>
       <c r="I18" s="78"/>
@@ -8805,7 +8811,7 @@
         <v>0.0</v>
       </c>
       <c r="L18" s="79" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M18" s="78"/>
       <c r="N18" s="78"/>
@@ -8817,32 +8823,32 @@
     </row>
     <row r="19">
       <c r="A19" s="80" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B19" s="72" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C19" s="73" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D19" s="74"/>
       <c r="E19" s="71" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F19" s="76" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="G19" s="76" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="H19" s="81"/>
       <c r="I19" s="78"/>
       <c r="J19" s="78"/>
       <c r="K19" s="71" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="L19" s="79" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="M19" s="78"/>
       <c r="N19" s="78"/>
@@ -8854,32 +8860,32 @@
     </row>
     <row r="20">
       <c r="A20" s="80" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B20" s="72" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="C20" s="73" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D20" s="74"/>
       <c r="E20" s="71" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F20" s="76" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="G20" s="76" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="H20" s="81"/>
       <c r="I20" s="78"/>
       <c r="J20" s="78"/>
       <c r="K20" s="71" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L20" s="79" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="M20" s="78"/>
       <c r="N20" s="78"/>
@@ -8891,32 +8897,32 @@
     </row>
     <row r="21">
       <c r="A21" s="80" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B21" s="72" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C21" s="73" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D21" s="74"/>
       <c r="E21" s="71" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F21" s="76" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="G21" s="76" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="H21" s="81"/>
       <c r="I21" s="78"/>
       <c r="J21" s="78"/>
       <c r="K21" s="71" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="L21" s="82" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="M21" s="78"/>
       <c r="N21" s="78"/>
@@ -8928,23 +8934,23 @@
     </row>
     <row r="22">
       <c r="A22" s="83" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B22" s="84" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C22" s="85" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D22" s="86"/>
       <c r="E22" s="87" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F22" s="88" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="G22" s="88" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="H22" s="89"/>
       <c r="I22" s="90"/>
@@ -8953,7 +8959,7 @@
         <v>0.0</v>
       </c>
       <c r="L22" s="92" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M22" s="90"/>
       <c r="N22" s="90"/>
@@ -8965,32 +8971,32 @@
     </row>
     <row r="23">
       <c r="A23" s="83" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B23" s="84" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="C23" s="85" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D23" s="86"/>
       <c r="E23" s="91" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F23" s="93" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="G23" s="93" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="H23" s="89"/>
       <c r="I23" s="90"/>
       <c r="J23" s="90"/>
       <c r="K23" s="91" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="L23" s="94" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="M23" s="90"/>
       <c r="N23" s="90"/>
@@ -9002,23 +9008,23 @@
     </row>
     <row r="24">
       <c r="A24" s="95" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B24" s="96" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C24" s="97" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D24" s="98"/>
       <c r="E24" s="99" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F24" s="100" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="G24" s="100" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="H24" s="101"/>
       <c r="I24" s="102"/>
@@ -9027,7 +9033,7 @@
         <v>0.0</v>
       </c>
       <c r="L24" s="104" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="M24" s="102"/>
       <c r="N24" s="102"/>
@@ -9039,32 +9045,32 @@
     </row>
     <row r="25">
       <c r="A25" s="95" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B25" s="96" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C25" s="97" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D25" s="98"/>
       <c r="E25" s="103" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F25" s="100" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="G25" s="100" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="H25" s="105"/>
       <c r="I25" s="102"/>
       <c r="J25" s="102"/>
       <c r="K25" s="106" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="L25" s="104" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="M25" s="102"/>
       <c r="N25" s="102"/>
@@ -9076,32 +9082,32 @@
     </row>
     <row r="26">
       <c r="A26" s="107" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B26" s="108" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C26" s="109" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D26" s="110"/>
       <c r="E26" s="111" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F26" s="112" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="G26" s="113" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="H26" s="114"/>
       <c r="I26" s="115"/>
       <c r="J26" s="115"/>
       <c r="K26" s="116" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="L26" s="117" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="M26" s="115"/>
       <c r="N26" s="115"/>
@@ -9113,32 +9119,32 @@
     </row>
     <row r="27">
       <c r="A27" s="118" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B27" s="108" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C27" s="109" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D27" s="119"/>
       <c r="E27" s="111" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F27" s="112" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="G27" s="118" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="H27" s="119"/>
       <c r="I27" s="115"/>
       <c r="J27" s="115"/>
       <c r="K27" s="116" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="L27" s="117" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="M27" s="115"/>
       <c r="N27" s="115"/>
@@ -9184,471 +9190,471 @@
         <v>1</v>
       </c>
       <c r="C1" s="122" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="122" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="E1" s="121" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="123" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B2" s="124" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C2" s="124" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D2" s="124"/>
       <c r="E2" s="36"/>
     </row>
     <row r="3">
       <c r="A3" s="123" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B3" s="124" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C3" s="124" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="D3" s="124"/>
       <c r="E3" s="36"/>
     </row>
     <row r="4">
       <c r="A4" s="123" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C4" s="124" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D4" s="124"/>
       <c r="E4" s="125" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="123" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C5" s="124" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="D5" s="124"/>
       <c r="E5" s="125" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="123" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C6" s="124" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="D6" s="124"/>
       <c r="E6" s="126" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="123" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C7" s="124" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="D7" s="124"/>
       <c r="E7" s="125" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="123" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="B8" s="124" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="C8" s="124" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="D8" s="124"/>
       <c r="E8" s="36"/>
     </row>
     <row r="9">
       <c r="A9" s="123" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B9" s="124" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C9" s="124" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="D9" s="124"/>
       <c r="E9" s="36"/>
     </row>
     <row r="10">
       <c r="A10" s="123" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="B10" s="127" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="C10" s="124" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="D10" s="124"/>
       <c r="E10" s="36"/>
     </row>
     <row r="11">
       <c r="A11" s="123" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B11" s="127" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="C11" s="124" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="D11" s="124"/>
       <c r="E11" s="36"/>
     </row>
     <row r="12">
       <c r="A12" s="123" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="B12" s="127" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="C12" s="124" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="D12" s="124"/>
       <c r="E12" s="36"/>
     </row>
     <row r="13">
       <c r="A13" s="123" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B13" s="127" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="C13" s="124" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="D13" s="124"/>
       <c r="E13" s="36"/>
     </row>
     <row r="14">
       <c r="A14" s="123" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B14" s="127" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C14" s="124" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="D14" s="124"/>
       <c r="E14" s="36"/>
     </row>
     <row r="15">
       <c r="A15" s="123" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B15" s="127" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="C15" s="124" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="D15" s="124"/>
       <c r="E15" s="36"/>
     </row>
     <row r="16">
       <c r="A16" s="123" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="B16" s="127" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="C16" s="124" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D16" s="124"/>
       <c r="E16" s="36"/>
     </row>
     <row r="17">
       <c r="A17" s="123" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B17" s="127" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C17" s="124" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="D17" s="124"/>
       <c r="E17" s="36"/>
     </row>
     <row r="18">
       <c r="A18" s="123" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B18" s="124" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="C18" s="124" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="D18" s="124"/>
       <c r="E18" s="36"/>
     </row>
     <row r="19">
       <c r="A19" s="123" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="B19" s="127" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="D19" s="128" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="E19" s="125" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="123" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="C20" s="129" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D20" s="129"/>
       <c r="E20" s="36"/>
     </row>
     <row r="21">
       <c r="A21" s="123" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B21" s="36" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C21" s="129" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="D21" s="129"/>
       <c r="E21" s="36"/>
     </row>
     <row r="22">
       <c r="A22" s="123" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="D22" s="129" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="E22" s="125" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="123" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="B23" s="124" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="C23" s="124" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D23" s="124"/>
       <c r="E23" s="125" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="123" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="B24" s="124" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="C24" s="124" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="D24" s="124"/>
       <c r="E24" s="36"/>
     </row>
     <row r="25">
       <c r="A25" s="123" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="B25" s="124" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C25" s="124" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="D25" s="124"/>
       <c r="E25" s="36"/>
     </row>
     <row r="26">
       <c r="A26" s="123" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="B26" s="124" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="C26" s="127" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="D26" s="127"/>
       <c r="E26" s="127"/>
     </row>
     <row r="27">
       <c r="A27" s="123" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="B27" s="124" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="C27" s="127" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="D27" s="127"/>
       <c r="E27" s="127"/>
     </row>
     <row r="28">
       <c r="A28" s="123" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="B28" s="124" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="C28" s="127" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="D28" s="127"/>
       <c r="E28" s="127"/>
     </row>
     <row r="29">
       <c r="A29" s="123" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="B29" s="124" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="C29" s="127" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="D29" s="127"/>
       <c r="E29" s="127"/>
     </row>
     <row r="30">
       <c r="A30" s="123" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="B30" s="124" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="C30" s="127" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="D30" s="127"/>
       <c r="E30" s="127"/>
     </row>
     <row r="31">
       <c r="A31" s="123" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="B31" s="124" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="C31" s="127" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="D31" s="127"/>
       <c r="E31" s="127"/>
     </row>
     <row r="32">
       <c r="A32" s="123" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="B32" s="124" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="C32" s="127" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="D32" s="127"/>
       <c r="E32" s="127"/>
     </row>
     <row r="33">
       <c r="A33" s="123" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="B33" s="124" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="C33" s="127" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="D33" s="127"/>
       <c r="E33" s="127"/>
     </row>
     <row r="34">
       <c r="A34" s="123" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="B34" s="124" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="C34" s="127" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="D34" s="127"/>
       <c r="E34" s="127"/>
     </row>
     <row r="35">
       <c r="A35" s="123" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="B35" s="124" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="C35" s="127" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="D35" s="127"/>
       <c r="E35" s="127"/>
@@ -9658,10 +9664,10 @@
         <v>54.0</v>
       </c>
       <c r="B36" s="131" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C36" s="36" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="D36" s="36"/>
       <c r="E36" s="36"/>
@@ -9671,10 +9677,10 @@
         <v>55.0</v>
       </c>
       <c r="B37" s="131" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="C37" s="36" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="D37" s="36"/>
       <c r="E37" s="36"/>
@@ -9684,10 +9690,10 @@
         <v>56.0</v>
       </c>
       <c r="B38" s="131" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="C38" s="36" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="D38" s="36"/>
       <c r="E38" s="36"/>
@@ -9697,218 +9703,218 @@
         <v>116.0</v>
       </c>
       <c r="B39" s="131" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C39" s="34" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="D39" s="34"/>
       <c r="E39" s="36"/>
     </row>
     <row r="40">
       <c r="A40" s="33" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="B40" s="131" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="C40" s="34" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D40" s="34"/>
       <c r="E40" s="36"/>
     </row>
     <row r="41">
       <c r="A41" s="33" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="B41" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="C41" s="132" t="s">
         <v>111</v>
-      </c>
-      <c r="C41" s="132" t="s">
-        <v>110</v>
       </c>
       <c r="D41" s="132"/>
       <c r="E41" s="36"/>
     </row>
     <row r="42">
       <c r="A42" s="38" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="B42" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="C42" s="132" t="s">
         <v>114</v>
-      </c>
-      <c r="C42" s="132" t="s">
-        <v>113</v>
       </c>
       <c r="D42" s="132"/>
       <c r="E42" s="36"/>
     </row>
     <row r="43">
       <c r="A43" s="33" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="B43" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="C43" s="132" t="s">
         <v>117</v>
-      </c>
-      <c r="C43" s="132" t="s">
-        <v>116</v>
       </c>
       <c r="D43" s="132"/>
       <c r="E43" s="36"/>
     </row>
     <row r="44">
       <c r="A44" s="38" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="B44" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="C44" s="132" t="s">
         <v>120</v>
-      </c>
-      <c r="C44" s="132" t="s">
-        <v>119</v>
       </c>
       <c r="D44" s="132"/>
       <c r="E44" s="36"/>
     </row>
     <row r="45">
       <c r="A45" s="33" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="B45" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="C45" s="132" t="s">
         <v>123</v>
-      </c>
-      <c r="C45" s="132" t="s">
-        <v>122</v>
       </c>
       <c r="D45" s="132"/>
       <c r="E45" s="36"/>
     </row>
     <row r="46">
       <c r="A46" s="38" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="B46" s="35" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C46" s="132" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="D46" s="132"/>
       <c r="E46" s="36"/>
     </row>
     <row r="47">
       <c r="A47" s="33" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="B47" s="35" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="C47" s="132" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="D47" s="132"/>
       <c r="E47" s="36"/>
     </row>
     <row r="48">
       <c r="A48" s="38" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="B48" s="35" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="C48" s="132" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="D48" s="132"/>
       <c r="E48" s="36"/>
     </row>
     <row r="49">
       <c r="A49" s="33" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B49" s="35" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C49" s="132" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="D49" s="132"/>
       <c r="E49" s="36"/>
     </row>
     <row r="50">
       <c r="A50" s="33" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="B50" s="35" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="C50" s="132" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="D50" s="132"/>
       <c r="E50" s="36"/>
     </row>
     <row r="51">
       <c r="A51" s="33" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="B51" s="35" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="C51" s="132" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="D51" s="132"/>
       <c r="E51" s="36"/>
     </row>
     <row r="52">
       <c r="A52" s="33" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="B52" s="35" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="C52" s="133" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="D52" s="134"/>
       <c r="E52" s="36"/>
     </row>
     <row r="53">
       <c r="A53" s="33" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B53" s="35" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="C53" s="133" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="D53" s="135"/>
       <c r="E53" s="36"/>
     </row>
     <row r="54">
       <c r="A54" s="33" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B54" s="35" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C54" s="133" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="D54" s="135"/>
       <c r="E54" s="36"/>
     </row>
     <row r="55">
       <c r="A55" s="38" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="C55" s="52" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D55" s="52"/>
       <c r="E55" s="36"/>
@@ -9944,188 +9950,188 @@
         <v>1</v>
       </c>
       <c r="C1" s="54" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="D1" s="54" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="E1" s="54" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="F1" s="54" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G1" s="56" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="13" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F2" s="136"/>
       <c r="G2" s="15"/>
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F3" s="136"/>
       <c r="G3" s="15"/>
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F4" s="136"/>
       <c r="G4" s="15"/>
     </row>
     <row r="5">
       <c r="A5" s="13" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F5" s="136"/>
       <c r="G5" s="15"/>
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F6" s="136"/>
       <c r="G6" s="15"/>
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F7" s="136"/>
       <c r="G7" s="15"/>
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F8" s="136"/>
       <c r="G8" s="15"/>
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F9" s="136"/>
       <c r="G9" s="15"/>
     </row>
     <row r="10">
       <c r="A10" s="13" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F10" s="136"/>
       <c r="G10" s="15"/>
@@ -10156,34 +10162,34 @@
         <v>1</v>
       </c>
       <c r="C1" s="56" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="54" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D2" s="15"/>
       <c r="F2" s="2" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="12" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D3" s="15"/>
       <c r="F3" s="2" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
     </row>
   </sheetData>
@@ -10225,92 +10231,92 @@
         <v>1</v>
       </c>
       <c r="C1" s="137" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D1" s="137" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="G1" s="137" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="K1" s="138" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="C2" s="139"/>
       <c r="D2" s="13"/>
       <c r="G2" s="140"/>
       <c r="I2" s="2" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="C3" s="140"/>
       <c r="D3" s="13"/>
       <c r="G3" s="140"/>
       <c r="I3" s="2" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
     </row>
     <row r="4" ht="20.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="C4" s="140"/>
       <c r="D4" s="13"/>
       <c r="E4" s="141"/>
       <c r="G4" s="142"/>
       <c r="I4" s="2" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="J4" s="143"/>
       <c r="K4" s="2" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="C5" s="140"/>
       <c r="D5" s="13"/>
@@ -10318,39 +10324,39 @@
       <c r="F5" s="142"/>
       <c r="G5" s="142"/>
       <c r="I5" s="2" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="J5" s="143"/>
       <c r="K5" s="2" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
     </row>
     <row r="6" ht="22.5" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="144"/>
       <c r="G6" s="140"/>
       <c r="I6" s="2" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
     </row>
     <row r="7" ht="22.5" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="144"/>
@@ -10358,13 +10364,13 @@
     </row>
     <row r="8" ht="22.5" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="144"/>
@@ -10392,16 +10398,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="32" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
@@ -10417,13 +10423,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
@@ -10464,13 +10470,13 @@
     </row>
     <row r="5">
       <c r="A5" s="15" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -10487,10 +10493,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -10505,10 +10511,10 @@
     <row r="7">
       <c r="A7" s="15"/>
       <c r="B7" s="15" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -10523,10 +10529,10 @@
     <row r="8">
       <c r="A8" s="15"/>
       <c r="B8" s="15" t="s">
+        <v>552</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>550</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>548</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -10541,10 +10547,10 @@
     <row r="9">
       <c r="A9" s="15"/>
       <c r="B9" s="15" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -10572,7 +10578,7 @@
     </row>
     <row r="11">
       <c r="A11" s="15" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="B11" s="145" t="s">
         <v>4</v>
@@ -10590,7 +10596,7 @@
     </row>
     <row r="12">
       <c r="A12" s="15" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="B12" s="146" t="s">
         <v>3</v>
@@ -10608,10 +10614,10 @@
     </row>
     <row r="13">
       <c r="A13" s="15" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="B13" s="146" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="L13" s="15"/>
     </row>
@@ -10641,38 +10647,38 @@
     </row>
     <row r="20">
       <c r="A20" s="147" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="B20" s="148" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="L20" s="15"/>
     </row>
     <row r="21">
       <c r="A21" s="147" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="B21" s="148" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="L21" s="15"/>
     </row>
     <row r="22">
       <c r="A22" s="147" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B22" s="149"/>
       <c r="L22" s="15"/>
     </row>
     <row r="23" hidden="1">
       <c r="A23" s="15" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="L23" s="15"/>
     </row>
     <row r="24" hidden="1">
       <c r="A24" s="15" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="L24" s="15"/>
     </row>
@@ -10729,42 +10735,42 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="151" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="C2" s="152" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="153" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="C3" s="152" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="154" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="C4" s="152" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="154" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="C5" s="152" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
spleen neuron 1 fix types and housing layers for axons
was causing parts to appear in csf and the connection to the final axon
terminal locations to be dropped because it was tagged as a dendrite
</commit_message>
<xml_diff>
--- a/models/spleen/source/spleen.xlsx
+++ b/models/spleen/source/spleen.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
     <author/>
   </authors>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
     <author/>
   </authors>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="628">
   <si>
     <t>id</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>sn_t5</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
   <si>
     <t>T6</t>
@@ -2242,7 +2245,7 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -2257,7 +2260,7 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -2994,60 +2997,60 @@
         <v>6</v>
       </c>
       <c r="D1" s="155" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E1" s="155" t="s">
         <v>9</v>
       </c>
       <c r="F1" s="155" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="2" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="39" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
   </sheetData>
@@ -3071,106 +3074,106 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="157" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="B2" s="158" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="157" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B3" s="159" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="157" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="B4" s="160" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="157" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="B5" s="160" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="157" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="B6" s="160" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="157" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="B7" s="160" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="157" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="B8" s="160" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="157" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="B9" s="160" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="157" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="B10" s="160" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="157" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B11" s="160" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="B12" s="152" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="B13" s="161" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
   </sheetData>
@@ -3214,97 +3217,97 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="163" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="163" t="s">
+        <v>613</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>612</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>613</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="163" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="163" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B5" s="164" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="163" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="B6" s="164" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="163" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B7" s="164" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="165"/>
       <c r="B8" s="164" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="165"/>
       <c r="B9" s="164" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="165"/>
       <c r="B10" s="164" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="165"/>
       <c r="B11" s="164" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="165"/>
       <c r="B12" s="164" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
     </row>
     <row r="13">
@@ -6397,7 +6400,9 @@
       <c r="M2" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="16"/>
+      <c r="N2" s="16" t="s">
+        <v>29</v>
+      </c>
       <c r="O2" s="15"/>
       <c r="P2" s="15"/>
       <c r="Q2" s="15"/>
@@ -6406,13 +6411,13 @@
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -6428,9 +6433,11 @@
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>
       <c r="M3" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" s="16"/>
+        <v>33</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>29</v>
+      </c>
       <c r="O3" s="15"/>
       <c r="P3" s="15"/>
       <c r="Q3" s="15"/>
@@ -6439,13 +6446,13 @@
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -6461,9 +6468,11 @@
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
       <c r="M4" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="N4" s="16"/>
+        <v>37</v>
+      </c>
+      <c r="N4" s="16" t="s">
+        <v>29</v>
+      </c>
       <c r="O4" s="15"/>
       <c r="P4" s="15"/>
       <c r="Q4" s="15"/>
@@ -6472,13 +6481,13 @@
     </row>
     <row r="5">
       <c r="A5" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -6494,9 +6503,11 @@
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
       <c r="M5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="N5" s="16"/>
+        <v>41</v>
+      </c>
+      <c r="N5" s="16" t="s">
+        <v>29</v>
+      </c>
       <c r="O5" s="15"/>
       <c r="P5" s="15"/>
       <c r="Q5" s="15"/>
@@ -6508,10 +6519,10 @@
         <v>27</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="19" t="b">
@@ -6521,13 +6532,13 @@
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
       <c r="I6" s="12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J6" s="20"/>
       <c r="K6" s="15"/>
       <c r="L6" s="15"/>
       <c r="M6" s="12"/>
-      <c r="N6" s="16"/>
+      <c r="N6" s="21"/>
       <c r="O6" s="15"/>
       <c r="P6" s="15"/>
       <c r="Q6" s="15"/>
@@ -6536,13 +6547,13 @@
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -6552,16 +6563,16 @@
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
       <c r="I7" s="12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J7" s="20"/>
       <c r="K7" s="15"/>
       <c r="L7" s="15"/>
-      <c r="M7" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="N7" s="21" t="s">
+      <c r="M7" s="16" t="s">
         <v>48</v>
+      </c>
+      <c r="N7" s="16" t="s">
+        <v>49</v>
       </c>
       <c r="O7" s="15"/>
       <c r="P7" s="15"/>
@@ -6571,13 +6582,13 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -6589,9 +6600,9 @@
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
       <c r="M8" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="N8" s="16"/>
+        <v>53</v>
+      </c>
+      <c r="N8" s="21"/>
       <c r="O8" s="15"/>
       <c r="P8" s="15"/>
       <c r="Q8" s="15"/>
@@ -6600,13 +6611,13 @@
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -6618,9 +6629,9 @@
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
       <c r="M9" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="N9" s="16"/>
+        <v>57</v>
+      </c>
+      <c r="N9" s="21"/>
       <c r="O9" s="15"/>
       <c r="P9" s="15"/>
       <c r="Q9" s="15"/>
@@ -6629,13 +6640,13 @@
     </row>
     <row r="10">
       <c r="A10" s="13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -6646,10 +6657,10 @@
       <c r="J10" s="20"/>
       <c r="K10" s="15"/>
       <c r="L10" s="15"/>
-      <c r="M10" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="N10" s="21"/>
+      <c r="M10" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="N10" s="16"/>
       <c r="O10" s="15"/>
       <c r="P10" s="15"/>
       <c r="Q10" s="15"/>
@@ -6658,13 +6669,13 @@
     </row>
     <row r="11">
       <c r="A11" s="13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
@@ -6676,9 +6687,9 @@
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
       <c r="M11" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="N11" s="16"/>
+        <v>64</v>
+      </c>
+      <c r="N11" s="21"/>
       <c r="O11" s="15"/>
       <c r="P11" s="15"/>
       <c r="Q11" s="15"/>
@@ -6687,13 +6698,13 @@
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
@@ -6705,9 +6716,9 @@
       <c r="K12" s="15"/>
       <c r="L12" s="15"/>
       <c r="M12" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="N12" s="16"/>
+        <v>68</v>
+      </c>
+      <c r="N12" s="21"/>
       <c r="O12" s="15"/>
       <c r="P12" s="15"/>
       <c r="Q12" s="15"/>
@@ -6716,28 +6727,28 @@
     </row>
     <row r="13">
       <c r="A13" s="13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
       <c r="I13" s="22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J13" s="20"/>
       <c r="K13" s="15"/>
       <c r="L13" s="15"/>
-      <c r="N13" s="16"/>
+      <c r="N13" s="21"/>
       <c r="O13" s="15"/>
       <c r="P13" s="15"/>
       <c r="Q13" s="15"/>
@@ -6746,18 +6757,18 @@
     </row>
     <row r="14">
       <c r="A14" s="13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
       <c r="F14" s="23" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
@@ -6765,10 +6776,10 @@
       <c r="K14" s="15"/>
       <c r="L14" s="15"/>
       <c r="M14" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="N14" s="21" t="s">
         <v>77</v>
+      </c>
+      <c r="N14" s="16" t="s">
+        <v>78</v>
       </c>
       <c r="O14" s="15"/>
       <c r="P14" s="15"/>
@@ -6778,18 +6789,18 @@
     </row>
     <row r="15">
       <c r="A15" s="13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="23" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
@@ -6798,10 +6809,10 @@
       <c r="K15" s="15"/>
       <c r="L15" s="15"/>
       <c r="M15" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="N15" s="21" t="s">
         <v>77</v>
+      </c>
+      <c r="N15" s="16" t="s">
+        <v>78</v>
       </c>
       <c r="O15" s="15"/>
       <c r="P15" s="15"/>
@@ -6811,18 +6822,18 @@
     </row>
     <row r="16">
       <c r="A16" s="24" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D16" s="26"/>
       <c r="E16" s="26"/>
       <c r="F16" s="27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G16" s="26"/>
       <c r="H16" s="26"/>
@@ -6831,10 +6842,10 @@
       <c r="K16" s="26"/>
       <c r="L16" s="26"/>
       <c r="M16" s="29" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="N16" s="30" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="O16" s="26"/>
       <c r="P16" s="26"/>
@@ -6844,13 +6855,13 @@
     </row>
     <row r="17">
       <c r="A17" s="13" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
@@ -6862,9 +6873,9 @@
       <c r="K17" s="15"/>
       <c r="L17" s="15"/>
       <c r="M17" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="N17" s="21"/>
+        <v>85</v>
+      </c>
+      <c r="N17" s="16"/>
       <c r="O17" s="15"/>
       <c r="P17" s="15"/>
       <c r="Q17" s="15"/>
@@ -6873,18 +6884,18 @@
     </row>
     <row r="18">
       <c r="A18" s="13" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
       <c r="F18" s="23" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
@@ -6893,10 +6904,10 @@
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
       <c r="M18" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="N18" s="21" t="s">
         <v>85</v>
+      </c>
+      <c r="N18" s="16" t="s">
+        <v>86</v>
       </c>
       <c r="O18" s="15"/>
       <c r="P18" s="15"/>
@@ -6906,13 +6917,13 @@
     </row>
     <row r="19">
       <c r="A19" s="13" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
@@ -6924,9 +6935,9 @@
       <c r="K19" s="15"/>
       <c r="L19" s="15"/>
       <c r="M19" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="N19" s="21"/>
+        <v>85</v>
+      </c>
+      <c r="N19" s="16"/>
       <c r="O19" s="15"/>
       <c r="P19" s="15"/>
       <c r="Q19" s="15"/>
@@ -6935,18 +6946,18 @@
     </row>
     <row r="20">
       <c r="A20" s="13" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="13" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
@@ -6955,10 +6966,10 @@
       <c r="K20" s="15"/>
       <c r="L20" s="15"/>
       <c r="M20" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="N20" s="21" t="s">
-        <v>85</v>
+        <v>100</v>
+      </c>
+      <c r="N20" s="16" t="s">
+        <v>86</v>
       </c>
       <c r="O20" s="15"/>
       <c r="P20" s="15"/>
@@ -6968,13 +6979,13 @@
     </row>
     <row r="21">
       <c r="A21" s="13" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="31"/>
@@ -6986,7 +6997,7 @@
       <c r="K21" s="15"/>
       <c r="L21" s="15"/>
       <c r="M21" s="15"/>
-      <c r="N21" s="16"/>
+      <c r="N21" s="21"/>
       <c r="O21" s="15"/>
       <c r="P21" s="15"/>
       <c r="Q21" s="15"/>
@@ -6995,13 +7006,13 @@
     </row>
     <row r="22">
       <c r="A22" s="18" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="31"/>
@@ -7009,13 +7020,13 @@
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
       <c r="I22" s="12" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J22" s="20"/>
       <c r="K22" s="15"/>
       <c r="L22" s="15"/>
       <c r="M22" s="12"/>
-      <c r="N22" s="21"/>
+      <c r="N22" s="16"/>
       <c r="O22" s="15"/>
       <c r="P22" s="15"/>
       <c r="Q22" s="15"/>
@@ -7024,13 +7035,13 @@
     </row>
     <row r="23">
       <c r="A23" s="33" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C23" s="35" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D23" s="36"/>
       <c r="E23" s="15"/>
@@ -7042,7 +7053,7 @@
       <c r="K23" s="15"/>
       <c r="L23" s="15"/>
       <c r="M23" s="15"/>
-      <c r="N23" s="16"/>
+      <c r="N23" s="21"/>
       <c r="O23" s="15"/>
       <c r="P23" s="15"/>
       <c r="Q23" s="15"/>
@@ -7051,13 +7062,13 @@
     </row>
     <row r="24">
       <c r="A24" s="33" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B24" s="37" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C24" s="35" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D24" s="36"/>
       <c r="E24" s="15"/>
@@ -7069,7 +7080,7 @@
       <c r="K24" s="15"/>
       <c r="L24" s="15"/>
       <c r="M24" s="15"/>
-      <c r="N24" s="16"/>
+      <c r="N24" s="21"/>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
       <c r="Q24" s="15"/>
@@ -7078,13 +7089,13 @@
     </row>
     <row r="25">
       <c r="A25" s="38" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B25" s="37" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C25" s="35" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D25" s="36"/>
       <c r="E25" s="15"/>
@@ -7096,7 +7107,7 @@
       <c r="K25" s="15"/>
       <c r="L25" s="15"/>
       <c r="M25" s="15"/>
-      <c r="N25" s="16"/>
+      <c r="N25" s="21"/>
       <c r="O25" s="15"/>
       <c r="P25" s="15"/>
       <c r="Q25" s="15"/>
@@ -7105,13 +7116,13 @@
     </row>
     <row r="26">
       <c r="A26" s="33" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B26" s="37" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C26" s="35" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D26" s="36"/>
       <c r="E26" s="15"/>
@@ -7123,7 +7134,7 @@
       <c r="K26" s="15"/>
       <c r="L26" s="15"/>
       <c r="M26" s="15"/>
-      <c r="N26" s="16"/>
+      <c r="N26" s="21"/>
       <c r="O26" s="15"/>
       <c r="P26" s="15"/>
       <c r="Q26" s="15"/>
@@ -7132,13 +7143,13 @@
     </row>
     <row r="27">
       <c r="A27" s="38" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B27" s="37" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C27" s="35" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D27" s="36"/>
       <c r="E27" s="15"/>
@@ -7150,7 +7161,7 @@
       <c r="K27" s="15"/>
       <c r="L27" s="15"/>
       <c r="M27" s="15"/>
-      <c r="N27" s="16"/>
+      <c r="N27" s="21"/>
       <c r="O27" s="15"/>
       <c r="P27" s="15"/>
       <c r="Q27" s="15"/>
@@ -7159,13 +7170,13 @@
     </row>
     <row r="28">
       <c r="A28" s="33" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C28" s="35" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D28" s="36"/>
       <c r="E28" s="15"/>
@@ -7177,7 +7188,7 @@
       <c r="K28" s="15"/>
       <c r="L28" s="15"/>
       <c r="M28" s="15"/>
-      <c r="N28" s="16"/>
+      <c r="N28" s="21"/>
       <c r="O28" s="15"/>
       <c r="P28" s="15"/>
       <c r="Q28" s="15"/>
@@ -7186,13 +7197,13 @@
     </row>
     <row r="29">
       <c r="A29" s="33" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B29" s="39" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C29" s="35" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D29" s="36"/>
       <c r="E29" s="15"/>
@@ -7204,7 +7215,7 @@
       <c r="K29" s="15"/>
       <c r="L29" s="15"/>
       <c r="M29" s="15"/>
-      <c r="N29" s="16"/>
+      <c r="N29" s="21"/>
       <c r="O29" s="15"/>
       <c r="P29" s="15"/>
       <c r="Q29" s="15"/>
@@ -7213,13 +7224,13 @@
     </row>
     <row r="30">
       <c r="A30" s="38" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B30" s="39" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C30" s="35" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D30" s="36"/>
       <c r="E30" s="15"/>
@@ -7230,7 +7241,7 @@
       <c r="J30" s="20"/>
       <c r="K30" s="15"/>
       <c r="M30" s="13" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="N30" s="12">
         <v>0.0</v>
@@ -7243,13 +7254,13 @@
     </row>
     <row r="31">
       <c r="A31" s="13" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
@@ -7260,7 +7271,7 @@
       <c r="J31" s="20"/>
       <c r="K31" s="15"/>
       <c r="M31" s="12" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="N31" s="12">
         <v>0.0</v>
@@ -7273,13 +7284,13 @@
     </row>
     <row r="32">
       <c r="A32" s="13" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D32" s="15"/>
       <c r="E32" s="31"/>
@@ -7287,12 +7298,12 @@
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
       <c r="I32" s="12" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="J32" s="20"/>
       <c r="K32" s="15"/>
       <c r="M32" s="15"/>
-      <c r="N32" s="16"/>
+      <c r="N32" s="21"/>
       <c r="O32" s="15"/>
       <c r="P32" s="15"/>
       <c r="Q32" s="15"/>
@@ -7301,13 +7312,13 @@
     </row>
     <row r="33">
       <c r="A33" s="13" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="31" t="b">
@@ -7317,13 +7328,13 @@
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
       <c r="I33" s="15" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J33" s="20"/>
       <c r="K33" s="15"/>
       <c r="L33" s="15"/>
       <c r="M33" s="15"/>
-      <c r="N33" s="16"/>
+      <c r="N33" s="21"/>
       <c r="O33" s="15"/>
       <c r="P33" s="15"/>
       <c r="Q33" s="15"/>
@@ -7332,13 +7343,13 @@
     </row>
     <row r="34">
       <c r="A34" s="40" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="41"/>
@@ -7350,7 +7361,7 @@
       <c r="K34" s="15"/>
       <c r="L34" s="15"/>
       <c r="M34" s="15"/>
-      <c r="N34" s="16"/>
+      <c r="N34" s="21"/>
       <c r="O34" s="15"/>
       <c r="P34" s="15"/>
       <c r="Q34" s="15"/>
@@ -7359,13 +7370,13 @@
     </row>
     <row r="35">
       <c r="A35" s="40" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B35" s="42" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D35" s="15"/>
       <c r="E35" s="41"/>
@@ -7377,7 +7388,7 @@
       <c r="K35" s="15"/>
       <c r="L35" s="15"/>
       <c r="M35" s="15"/>
-      <c r="N35" s="16"/>
+      <c r="N35" s="21"/>
       <c r="O35" s="15"/>
       <c r="P35" s="15"/>
       <c r="Q35" s="15"/>
@@ -7386,31 +7397,31 @@
     </row>
     <row r="36">
       <c r="A36" s="43" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D36" s="15"/>
       <c r="E36" s="41" t="b">
         <v>1</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G36" s="15"/>
       <c r="H36" s="15"/>
       <c r="I36" s="15" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J36" s="20"/>
       <c r="K36" s="15"/>
       <c r="L36" s="15"/>
       <c r="M36" s="15"/>
-      <c r="N36" s="16"/>
+      <c r="N36" s="21"/>
       <c r="O36" s="15"/>
       <c r="P36" s="15"/>
       <c r="Q36" s="15"/>
@@ -7419,13 +7430,13 @@
     </row>
     <row r="37">
       <c r="A37" s="43" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D37" s="15"/>
       <c r="E37" s="41" t="b">
@@ -7437,13 +7448,13 @@
       <c r="G37" s="15"/>
       <c r="H37" s="15"/>
       <c r="I37" s="15" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J37" s="20"/>
       <c r="K37" s="15"/>
       <c r="L37" s="15"/>
       <c r="M37" s="15"/>
-      <c r="N37" s="16"/>
+      <c r="N37" s="21"/>
       <c r="O37" s="15"/>
       <c r="P37" s="15"/>
       <c r="Q37" s="15"/>
@@ -7452,31 +7463,31 @@
     </row>
     <row r="38">
       <c r="A38" s="43" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D38" s="15"/>
       <c r="E38" s="41" t="b">
         <v>1</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G38" s="15"/>
       <c r="H38" s="15"/>
       <c r="I38" s="15" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J38" s="20"/>
       <c r="K38" s="15"/>
       <c r="L38" s="15"/>
       <c r="M38" s="15"/>
-      <c r="N38" s="16"/>
+      <c r="N38" s="21"/>
       <c r="O38" s="15"/>
       <c r="P38" s="15"/>
       <c r="Q38" s="15"/>
@@ -7485,13 +7496,13 @@
     </row>
     <row r="39">
       <c r="A39" s="43" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D39" s="15"/>
       <c r="E39" s="41" t="b">
@@ -7503,13 +7514,13 @@
       <c r="G39" s="15"/>
       <c r="H39" s="15"/>
       <c r="I39" s="15" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J39" s="20"/>
       <c r="K39" s="15"/>
       <c r="L39" s="15"/>
       <c r="M39" s="15"/>
-      <c r="N39" s="16"/>
+      <c r="N39" s="21"/>
       <c r="O39" s="15"/>
       <c r="P39" s="15"/>
       <c r="Q39" s="15"/>
@@ -7518,13 +7529,13 @@
     </row>
     <row r="40">
       <c r="A40" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B40" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D40" s="15"/>
       <c r="E40" s="15"/>
@@ -7533,29 +7544,29 @@
       <c r="H40" s="15"/>
       <c r="I40" s="15"/>
       <c r="J40" s="13" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K40" s="15"/>
       <c r="L40" s="15"/>
       <c r="M40" s="15"/>
-      <c r="N40" s="16"/>
+      <c r="N40" s="21"/>
       <c r="O40" s="15"/>
       <c r="P40" s="15"/>
       <c r="Q40" s="15"/>
       <c r="R40" s="15"/>
       <c r="S40" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B41" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D41" s="15"/>
       <c r="E41" s="15"/>
@@ -7564,12 +7575,12 @@
       <c r="H41" s="15"/>
       <c r="I41" s="15"/>
       <c r="J41" s="13" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K41" s="15"/>
       <c r="L41" s="15"/>
       <c r="M41" s="15"/>
-      <c r="N41" s="16"/>
+      <c r="N41" s="21"/>
       <c r="O41" s="15"/>
       <c r="P41" s="15"/>
       <c r="Q41" s="15"/>
@@ -7577,13 +7588,13 @@
     </row>
     <row r="42">
       <c r="A42" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B42" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D42" s="15"/>
       <c r="E42" s="15"/>
@@ -7592,12 +7603,12 @@
       <c r="H42" s="15"/>
       <c r="I42" s="15"/>
       <c r="J42" s="13" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K42" s="15"/>
       <c r="L42" s="15"/>
       <c r="M42" s="15"/>
-      <c r="N42" s="16"/>
+      <c r="N42" s="21"/>
       <c r="O42" s="15"/>
       <c r="P42" s="15"/>
       <c r="Q42" s="15"/>
@@ -7608,10 +7619,10 @@
         <v>28</v>
       </c>
       <c r="B43" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D43" s="15"/>
       <c r="E43" s="15"/>
@@ -7620,12 +7631,12 @@
       <c r="H43" s="15"/>
       <c r="I43" s="15"/>
       <c r="J43" s="13" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K43" s="15"/>
       <c r="L43" s="15"/>
       <c r="M43" s="15"/>
-      <c r="N43" s="16"/>
+      <c r="N43" s="21"/>
       <c r="O43" s="15"/>
       <c r="P43" s="15"/>
       <c r="Q43" s="15"/>
@@ -7633,13 +7644,13 @@
     </row>
     <row r="44">
       <c r="A44" s="13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B44" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D44" s="15"/>
       <c r="E44" s="15"/>
@@ -7648,29 +7659,29 @@
       <c r="H44" s="15"/>
       <c r="I44" s="15"/>
       <c r="J44" s="13" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K44" s="15"/>
       <c r="L44" s="15"/>
       <c r="M44" s="15"/>
-      <c r="N44" s="16"/>
+      <c r="N44" s="21"/>
       <c r="O44" s="15"/>
       <c r="P44" s="15"/>
       <c r="Q44" s="15"/>
       <c r="R44" s="15"/>
       <c r="S44" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="45" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B45" s="46" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C45" s="47" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D45" s="48"/>
       <c r="E45" s="48"/>
@@ -7679,7 +7690,7 @@
       <c r="H45" s="48"/>
       <c r="I45" s="48"/>
       <c r="J45" s="45" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K45" s="48"/>
       <c r="L45" s="48"/>
@@ -7690,18 +7701,18 @@
       <c r="Q45" s="48"/>
       <c r="R45" s="48"/>
       <c r="S45" s="51" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="45" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B46" s="46" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C46" s="47" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D46" s="48"/>
       <c r="E46" s="48"/>
@@ -7710,7 +7721,7 @@
       <c r="H46" s="48"/>
       <c r="I46" s="48"/>
       <c r="J46" s="45" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K46" s="48"/>
       <c r="L46" s="48"/>
@@ -7721,18 +7732,18 @@
       <c r="Q46" s="48"/>
       <c r="R46" s="48"/>
       <c r="S46" s="51" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B47" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D47" s="15"/>
       <c r="E47" s="15"/>
@@ -7741,29 +7752,29 @@
       <c r="H47" s="15"/>
       <c r="I47" s="15"/>
       <c r="J47" s="13" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K47" s="15"/>
       <c r="L47" s="15"/>
       <c r="M47" s="15"/>
-      <c r="N47" s="16"/>
+      <c r="N47" s="21"/>
       <c r="O47" s="15"/>
       <c r="P47" s="15"/>
       <c r="Q47" s="15"/>
       <c r="R47" s="15"/>
       <c r="S47" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="13" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B48" s="52" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D48" s="15"/>
       <c r="E48" s="12" t="b">
@@ -7773,12 +7784,12 @@
       <c r="G48" s="15"/>
       <c r="H48" s="15"/>
       <c r="I48" s="12" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="J48" s="20"/>
       <c r="L48" s="15"/>
       <c r="M48" s="15"/>
-      <c r="N48" s="16"/>
+      <c r="N48" s="21"/>
       <c r="O48" s="15"/>
       <c r="P48" s="15"/>
       <c r="Q48" s="15"/>
@@ -7787,13 +7798,13 @@
     </row>
     <row r="49">
       <c r="A49" s="13" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B49" s="52" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D49" s="15"/>
       <c r="E49" s="12" t="b">
@@ -7803,12 +7814,12 @@
       <c r="G49" s="15"/>
       <c r="H49" s="15"/>
       <c r="I49" s="12" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="J49" s="20"/>
       <c r="L49" s="15"/>
       <c r="M49" s="15"/>
-      <c r="N49" s="16"/>
+      <c r="N49" s="21"/>
       <c r="O49" s="15"/>
       <c r="P49" s="15"/>
       <c r="Q49" s="15"/>
@@ -7817,13 +7828,13 @@
     </row>
     <row r="50">
       <c r="A50" s="13" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B50" s="52" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D50" s="15"/>
       <c r="E50" s="12" t="b">
@@ -7833,12 +7844,12 @@
       <c r="G50" s="15"/>
       <c r="H50" s="15"/>
       <c r="I50" s="12" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="J50" s="20"/>
       <c r="L50" s="15"/>
       <c r="M50" s="15"/>
-      <c r="N50" s="16"/>
+      <c r="N50" s="21"/>
       <c r="O50" s="15"/>
       <c r="P50" s="15"/>
       <c r="Q50" s="15"/>
@@ -7847,13 +7858,13 @@
     </row>
     <row r="51">
       <c r="A51" s="13" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B51" s="52" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D51" s="15"/>
       <c r="E51" s="12" t="b">
@@ -7863,12 +7874,12 @@
       <c r="G51" s="15"/>
       <c r="H51" s="15"/>
       <c r="I51" s="12" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="J51" s="20"/>
       <c r="L51" s="15"/>
       <c r="M51" s="15"/>
-      <c r="N51" s="16"/>
+      <c r="N51" s="21"/>
       <c r="O51" s="15"/>
       <c r="P51" s="15"/>
       <c r="Q51" s="15"/>
@@ -7877,13 +7888,13 @@
     </row>
     <row r="52">
       <c r="A52" s="13" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B52" s="52" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D52" s="15"/>
       <c r="E52" s="15"/>
@@ -7893,11 +7904,11 @@
       <c r="I52" s="15"/>
       <c r="J52" s="20"/>
       <c r="K52" s="53" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="L52" s="15"/>
       <c r="M52" s="15"/>
-      <c r="N52" s="16"/>
+      <c r="N52" s="21"/>
       <c r="O52" s="15"/>
       <c r="P52" s="15"/>
       <c r="Q52" s="15"/>
@@ -7906,13 +7917,13 @@
     </row>
     <row r="53">
       <c r="A53" s="13" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B53" s="52" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D53" s="15"/>
       <c r="E53" s="12" t="b">
@@ -7922,12 +7933,12 @@
       <c r="G53" s="15"/>
       <c r="H53" s="15"/>
       <c r="I53" s="12" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="J53" s="20"/>
       <c r="L53" s="15"/>
       <c r="M53" s="15"/>
-      <c r="N53" s="16"/>
+      <c r="N53" s="21"/>
       <c r="O53" s="15"/>
       <c r="P53" s="15"/>
       <c r="Q53" s="15"/>
@@ -7936,13 +7947,13 @@
     </row>
     <row r="54">
       <c r="A54" s="13" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B54" s="52" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D54" s="15"/>
       <c r="E54" s="15"/>
@@ -7950,12 +7961,12 @@
       <c r="G54" s="15"/>
       <c r="H54" s="15"/>
       <c r="I54" s="12" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="J54" s="20"/>
       <c r="L54" s="15"/>
       <c r="M54" s="15"/>
-      <c r="N54" s="16"/>
+      <c r="N54" s="21"/>
       <c r="O54" s="15"/>
       <c r="P54" s="15"/>
       <c r="Q54" s="15"/>
@@ -7964,13 +7975,13 @@
     </row>
     <row r="55">
       <c r="A55" s="13" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B55" s="52" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D55" s="15"/>
       <c r="E55" s="15"/>
@@ -7978,12 +7989,12 @@
       <c r="G55" s="15"/>
       <c r="H55" s="15"/>
       <c r="I55" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="J55" s="20"/>
       <c r="L55" s="15"/>
       <c r="M55" s="15"/>
-      <c r="N55" s="16"/>
+      <c r="N55" s="21"/>
       <c r="O55" s="15"/>
       <c r="P55" s="15"/>
       <c r="Q55" s="15"/>
@@ -7992,13 +8003,13 @@
     </row>
     <row r="56">
       <c r="A56" s="13" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B56" s="52" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D56" s="15"/>
       <c r="E56" s="15"/>
@@ -8006,12 +8017,12 @@
       <c r="G56" s="15"/>
       <c r="H56" s="15"/>
       <c r="I56" s="12" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="J56" s="20"/>
       <c r="L56" s="15"/>
       <c r="M56" s="15"/>
-      <c r="N56" s="16"/>
+      <c r="N56" s="21"/>
       <c r="O56" s="15"/>
       <c r="P56" s="15"/>
       <c r="Q56" s="15"/>
@@ -8020,13 +8031,13 @@
     </row>
     <row r="57">
       <c r="A57" s="13" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B57" s="52" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D57" s="15"/>
       <c r="E57" s="12" t="b">
@@ -8036,12 +8047,12 @@
       <c r="G57" s="15"/>
       <c r="H57" s="15"/>
       <c r="I57" s="12" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="J57" s="20"/>
       <c r="L57" s="15"/>
       <c r="M57" s="15"/>
-      <c r="N57" s="16"/>
+      <c r="N57" s="21"/>
       <c r="O57" s="15"/>
       <c r="P57" s="15"/>
       <c r="Q57" s="15"/>
@@ -8050,13 +8061,13 @@
     </row>
     <row r="58">
       <c r="A58" s="13" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B58" s="52" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D58" s="15"/>
       <c r="E58" s="15"/>
@@ -8064,12 +8075,12 @@
       <c r="G58" s="15"/>
       <c r="H58" s="15"/>
       <c r="I58" s="12" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="J58" s="20"/>
       <c r="L58" s="15"/>
       <c r="M58" s="15"/>
-      <c r="N58" s="16"/>
+      <c r="N58" s="21"/>
       <c r="O58" s="15"/>
       <c r="P58" s="15"/>
       <c r="Q58" s="15"/>
@@ -8078,13 +8089,13 @@
     </row>
     <row r="59">
       <c r="A59" s="13" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B59" s="52" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D59" s="15"/>
       <c r="E59" s="15"/>
@@ -8092,12 +8103,12 @@
       <c r="G59" s="15"/>
       <c r="H59" s="15"/>
       <c r="I59" s="12" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="J59" s="20"/>
       <c r="L59" s="15"/>
       <c r="M59" s="15"/>
-      <c r="N59" s="16"/>
+      <c r="N59" s="21"/>
       <c r="O59" s="15"/>
       <c r="P59" s="15"/>
       <c r="Q59" s="15"/>
@@ -8106,13 +8117,13 @@
     </row>
     <row r="60">
       <c r="A60" s="13" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D60" s="15"/>
       <c r="E60" s="15"/>
@@ -8123,7 +8134,7 @@
       <c r="J60" s="20"/>
       <c r="L60" s="15"/>
       <c r="M60" s="15"/>
-      <c r="N60" s="16"/>
+      <c r="N60" s="21"/>
       <c r="O60" s="15"/>
       <c r="P60" s="15"/>
       <c r="Q60" s="15"/>
@@ -8177,43 +8188,43 @@
         <v>6</v>
       </c>
       <c r="D1" s="54" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E1" s="54" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="F1" s="54" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G1" s="54" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H1" s="54" t="s">
         <v>10</v>
       </c>
       <c r="I1" s="54" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="J1" s="57" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K1" s="54" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="L1" s="58" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="M1" s="56" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="N1" s="54" t="s">
         <v>21</v>
       </c>
       <c r="O1" s="54" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="P1" s="32" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="Q1" s="32"/>
       <c r="R1" s="32"/>
@@ -8221,14 +8232,14 @@
     </row>
     <row r="2">
       <c r="A2" s="13" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C2" s="60"/>
       <c r="D2" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E2" s="43"/>
       <c r="F2" s="12"/>
@@ -8240,7 +8251,7 @@
       <c r="M2" s="15"/>
       <c r="N2" s="15"/>
       <c r="O2" s="12" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="P2" s="31" t="b">
         <v>1</v>
@@ -8251,16 +8262,16 @@
     </row>
     <row r="3">
       <c r="A3" s="18" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B3" s="61" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="12" t="s">
         <v>104</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>103</v>
       </c>
       <c r="E3" s="31"/>
       <c r="F3" s="32"/>
@@ -8271,9 +8282,9 @@
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>
       <c r="M3" s="12"/>
-      <c r="N3" s="21"/>
+      <c r="N3" s="16"/>
       <c r="O3" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="P3" s="12" t="b">
         <v>1</v>
@@ -8284,35 +8295,35 @@
     </row>
     <row r="4">
       <c r="A4" s="18" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B4" s="61" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="12"/>
       <c r="E4" s="13" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="H4" s="15"/>
       <c r="I4" s="12"/>
       <c r="J4" s="20"/>
       <c r="K4" s="15"/>
       <c r="L4" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="N4" s="21"/>
+        <v>86</v>
+      </c>
+      <c r="N4" s="16"/>
       <c r="O4" s="12" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="P4" s="12" t="b">
         <v>1</v>
@@ -8323,33 +8334,33 @@
     </row>
     <row r="5">
       <c r="A5" s="18" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B5" s="61" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="12"/>
       <c r="E5" s="13" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="H5" s="15"/>
       <c r="I5" s="12"/>
       <c r="J5" s="20"/>
       <c r="K5" s="15"/>
       <c r="L5" s="12" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="N5" s="21"/>
+        <v>78</v>
+      </c>
+      <c r="N5" s="16"/>
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
       <c r="Q5" s="15"/>
@@ -8358,33 +8369,33 @@
     </row>
     <row r="6">
       <c r="A6" s="18" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B6" s="61" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="12"/>
       <c r="E6" s="13" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H6" s="15"/>
       <c r="I6" s="12"/>
       <c r="J6" s="20"/>
       <c r="K6" s="15"/>
       <c r="L6" s="12" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="N6" s="21"/>
+        <v>78</v>
+      </c>
+      <c r="N6" s="16"/>
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
       <c r="Q6" s="15"/>
@@ -8393,30 +8404,30 @@
     </row>
     <row r="7">
       <c r="A7" s="18" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B7" s="61" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C7" s="60"/>
       <c r="E7" s="13" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
       <c r="K7" s="61"/>
       <c r="L7" s="13" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="N7" s="15"/>
       <c r="O7" s="15"/>
@@ -8427,30 +8438,30 @@
     </row>
     <row r="8">
       <c r="A8" s="18" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B8" s="61" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C8" s="60"/>
       <c r="E8" s="13" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="61"/>
       <c r="L8" s="13" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N8" s="15"/>
       <c r="O8" s="15"/>
@@ -8461,32 +8472,32 @@
     </row>
     <row r="9">
       <c r="A9" s="62" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B9" s="63" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C9" s="64" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D9" s="65"/>
       <c r="E9" s="62" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F9" s="66" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G9" s="66" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H9" s="67"/>
       <c r="I9" s="68"/>
       <c r="J9" s="68"/>
       <c r="K9" s="69" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="L9" s="62" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="M9" s="68"/>
       <c r="N9" s="68"/>
@@ -8498,32 +8509,32 @@
     </row>
     <row r="10">
       <c r="A10" s="62" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B10" s="63" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C10" s="64" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D10" s="65"/>
       <c r="E10" s="62" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F10" s="66" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="G10" s="66" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H10" s="68"/>
       <c r="I10" s="68"/>
       <c r="J10" s="68"/>
       <c r="K10" s="69" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="L10" s="62" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M10" s="68"/>
       <c r="N10" s="68"/>
@@ -8535,32 +8546,32 @@
     </row>
     <row r="11">
       <c r="A11" s="62" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B11" s="63" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C11" s="64" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D11" s="65"/>
       <c r="E11" s="62" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F11" s="66" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G11" s="66" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H11" s="67"/>
       <c r="I11" s="68"/>
       <c r="J11" s="68"/>
       <c r="K11" s="69" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="L11" s="62" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="M11" s="68"/>
       <c r="N11" s="68"/>
@@ -8572,32 +8583,32 @@
     </row>
     <row r="12">
       <c r="A12" s="62" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B12" s="63" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C12" s="64" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D12" s="65"/>
       <c r="E12" s="62" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F12" s="66" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G12" s="66" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H12" s="67"/>
       <c r="I12" s="68"/>
       <c r="J12" s="68"/>
       <c r="K12" s="69" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="L12" s="62" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="M12" s="68"/>
       <c r="N12" s="68"/>
@@ -8609,20 +8620,20 @@
     </row>
     <row r="13">
       <c r="A13" s="62" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B13" s="63" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C13" s="64" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D13" s="65"/>
       <c r="E13" s="70" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F13" s="66" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G13" s="65"/>
       <c r="H13" s="67"/>
@@ -8632,7 +8643,7 @@
         <v>2.0</v>
       </c>
       <c r="L13" s="62" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M13" s="68"/>
       <c r="N13" s="68"/>
@@ -8644,20 +8655,20 @@
     </row>
     <row r="14">
       <c r="A14" s="62" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B14" s="63" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C14" s="64" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D14" s="65"/>
       <c r="E14" s="70" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F14" s="66" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="G14" s="65"/>
       <c r="H14" s="67"/>
@@ -8667,7 +8678,7 @@
         <v>2.0</v>
       </c>
       <c r="L14" s="62" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M14" s="68"/>
       <c r="N14" s="68"/>
@@ -8679,20 +8690,20 @@
     </row>
     <row r="15">
       <c r="A15" s="62" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C15" s="64" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D15" s="65"/>
       <c r="E15" s="70" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F15" s="66" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="G15" s="65"/>
       <c r="H15" s="68"/>
@@ -8702,7 +8713,7 @@
         <v>2.0</v>
       </c>
       <c r="L15" s="62" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M15" s="68"/>
       <c r="N15" s="68"/>
@@ -8714,20 +8725,20 @@
     </row>
     <row r="16">
       <c r="A16" s="62" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C16" s="64" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D16" s="65"/>
       <c r="E16" s="70" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F16" s="66" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G16" s="65"/>
       <c r="H16" s="67"/>
@@ -8749,32 +8760,32 @@
     </row>
     <row r="17">
       <c r="A17" s="62" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C17" s="64" t="s">
-        <v>275</v>
+        <v>257</v>
       </c>
       <c r="D17" s="65"/>
       <c r="E17" s="62" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F17" s="66" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="G17" s="66" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="H17" s="67"/>
       <c r="I17" s="68"/>
       <c r="J17" s="68"/>
       <c r="K17" s="69" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="L17" s="62" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="M17" s="68"/>
       <c r="N17" s="68"/>
@@ -8786,23 +8797,23 @@
     </row>
     <row r="18">
       <c r="A18" s="71" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B18" s="72" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C18" s="73" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D18" s="74"/>
       <c r="E18" s="75" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F18" s="76" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G18" s="76" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="H18" s="77"/>
       <c r="I18" s="78"/>
@@ -8811,7 +8822,7 @@
         <v>0.0</v>
       </c>
       <c r="L18" s="79" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M18" s="78"/>
       <c r="N18" s="78"/>
@@ -8823,32 +8834,32 @@
     </row>
     <row r="19">
       <c r="A19" s="80" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B19" s="72" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C19" s="73" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D19" s="74"/>
       <c r="E19" s="71" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F19" s="76" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="G19" s="76" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H19" s="81"/>
       <c r="I19" s="78"/>
       <c r="J19" s="78"/>
       <c r="K19" s="71" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="L19" s="79" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="M19" s="78"/>
       <c r="N19" s="78"/>
@@ -8860,32 +8871,32 @@
     </row>
     <row r="20">
       <c r="A20" s="80" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B20" s="72" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C20" s="73" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D20" s="74"/>
       <c r="E20" s="71" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F20" s="76" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G20" s="76" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="H20" s="81"/>
       <c r="I20" s="78"/>
       <c r="J20" s="78"/>
       <c r="K20" s="71" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="L20" s="79" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="M20" s="78"/>
       <c r="N20" s="78"/>
@@ -8897,32 +8908,32 @@
     </row>
     <row r="21">
       <c r="A21" s="80" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B21" s="72" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C21" s="73" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D21" s="74"/>
       <c r="E21" s="71" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F21" s="76" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G21" s="76" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="H21" s="81"/>
       <c r="I21" s="78"/>
       <c r="J21" s="78"/>
       <c r="K21" s="71" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="L21" s="82" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="M21" s="78"/>
       <c r="N21" s="78"/>
@@ -8934,23 +8945,23 @@
     </row>
     <row r="22">
       <c r="A22" s="83" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B22" s="84" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C22" s="85" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D22" s="86"/>
       <c r="E22" s="87" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F22" s="88" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="G22" s="88" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="H22" s="89"/>
       <c r="I22" s="90"/>
@@ -8959,7 +8970,7 @@
         <v>0.0</v>
       </c>
       <c r="L22" s="92" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="M22" s="90"/>
       <c r="N22" s="90"/>
@@ -8971,32 +8982,32 @@
     </row>
     <row r="23">
       <c r="A23" s="83" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B23" s="84" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C23" s="85" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D23" s="86"/>
       <c r="E23" s="91" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F23" s="93" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="G23" s="93" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="H23" s="89"/>
       <c r="I23" s="90"/>
       <c r="J23" s="90"/>
       <c r="K23" s="91" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="L23" s="94" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="M23" s="90"/>
       <c r="N23" s="90"/>
@@ -9008,23 +9019,23 @@
     </row>
     <row r="24">
       <c r="A24" s="95" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B24" s="96" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C24" s="97" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D24" s="98"/>
       <c r="E24" s="99" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F24" s="100" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="G24" s="100" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="H24" s="101"/>
       <c r="I24" s="102"/>
@@ -9033,7 +9044,7 @@
         <v>0.0</v>
       </c>
       <c r="L24" s="104" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M24" s="102"/>
       <c r="N24" s="102"/>
@@ -9045,32 +9056,32 @@
     </row>
     <row r="25">
       <c r="A25" s="95" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B25" s="96" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C25" s="97" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D25" s="98"/>
       <c r="E25" s="103" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F25" s="100" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="G25" s="100" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="H25" s="105"/>
       <c r="I25" s="102"/>
       <c r="J25" s="102"/>
       <c r="K25" s="106" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="L25" s="104" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="M25" s="102"/>
       <c r="N25" s="102"/>
@@ -9082,32 +9093,32 @@
     </row>
     <row r="26">
       <c r="A26" s="107" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B26" s="108" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C26" s="109" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D26" s="110"/>
       <c r="E26" s="111" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F26" s="112" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="G26" s="113" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="H26" s="114"/>
       <c r="I26" s="115"/>
       <c r="J26" s="115"/>
       <c r="K26" s="116" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="L26" s="117" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="M26" s="115"/>
       <c r="N26" s="115"/>
@@ -9119,32 +9130,32 @@
     </row>
     <row r="27">
       <c r="A27" s="118" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B27" s="108" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C27" s="109" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D27" s="119"/>
       <c r="E27" s="111" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F27" s="112" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="G27" s="118" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="H27" s="119"/>
       <c r="I27" s="115"/>
       <c r="J27" s="115"/>
       <c r="K27" s="116" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="L27" s="117" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="M27" s="115"/>
       <c r="N27" s="115"/>
@@ -9193,7 +9204,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="122" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E1" s="121" t="s">
         <v>14</v>
@@ -9201,460 +9212,460 @@
     </row>
     <row r="2">
       <c r="A2" s="123" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B2" s="124" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C2" s="124" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D2" s="124"/>
       <c r="E2" s="36"/>
     </row>
     <row r="3">
       <c r="A3" s="123" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B3" s="124" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C3" s="124" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D3" s="124"/>
       <c r="E3" s="36"/>
     </row>
     <row r="4">
       <c r="A4" s="123" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C4" s="124" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D4" s="124"/>
       <c r="E4" s="125" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="123" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C5" s="124" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D5" s="124"/>
       <c r="E5" s="125" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="123" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C6" s="124" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D6" s="124"/>
       <c r="E6" s="126" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="123" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C7" s="124" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D7" s="124"/>
       <c r="E7" s="125" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="123" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B8" s="124" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C8" s="124" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D8" s="124"/>
       <c r="E8" s="36"/>
     </row>
     <row r="9">
       <c r="A9" s="123" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B9" s="124" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C9" s="124" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D9" s="124"/>
       <c r="E9" s="36"/>
     </row>
     <row r="10">
       <c r="A10" s="123" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B10" s="127" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C10" s="124" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D10" s="124"/>
       <c r="E10" s="36"/>
     </row>
     <row r="11">
       <c r="A11" s="123" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B11" s="127" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C11" s="124" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D11" s="124"/>
       <c r="E11" s="36"/>
     </row>
     <row r="12">
       <c r="A12" s="123" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B12" s="127" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C12" s="124" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D12" s="124"/>
       <c r="E12" s="36"/>
     </row>
     <row r="13">
       <c r="A13" s="123" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B13" s="127" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C13" s="124" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D13" s="124"/>
       <c r="E13" s="36"/>
     </row>
     <row r="14">
       <c r="A14" s="123" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B14" s="127" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C14" s="124" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D14" s="124"/>
       <c r="E14" s="36"/>
     </row>
     <row r="15">
       <c r="A15" s="123" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B15" s="127" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C15" s="124" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D15" s="124"/>
       <c r="E15" s="36"/>
     </row>
     <row r="16">
       <c r="A16" s="123" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B16" s="127" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C16" s="124" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D16" s="124"/>
       <c r="E16" s="36"/>
     </row>
     <row r="17">
       <c r="A17" s="123" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B17" s="127" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C17" s="124" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D17" s="124"/>
       <c r="E17" s="36"/>
     </row>
     <row r="18">
       <c r="A18" s="123" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B18" s="124" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C18" s="124" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D18" s="124"/>
       <c r="E18" s="36"/>
     </row>
     <row r="19">
       <c r="A19" s="123" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B19" s="127" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D19" s="128" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E19" s="125" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="123" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C20" s="129" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D20" s="129"/>
       <c r="E20" s="36"/>
     </row>
     <row r="21">
       <c r="A21" s="123" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B21" s="36" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C21" s="129" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D21" s="129"/>
       <c r="E21" s="36"/>
     </row>
     <row r="22">
       <c r="A22" s="123" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D22" s="129" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="E22" s="125" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="123" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B23" s="124" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C23" s="124" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D23" s="124"/>
       <c r="E23" s="125" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="123" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B24" s="124" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C24" s="124" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D24" s="124"/>
       <c r="E24" s="36"/>
     </row>
     <row r="25">
       <c r="A25" s="123" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B25" s="124" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C25" s="124" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D25" s="124"/>
       <c r="E25" s="36"/>
     </row>
     <row r="26">
       <c r="A26" s="123" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B26" s="124" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C26" s="127" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D26" s="127"/>
       <c r="E26" s="127"/>
     </row>
     <row r="27">
       <c r="A27" s="123" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B27" s="124" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C27" s="127" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D27" s="127"/>
       <c r="E27" s="127"/>
     </row>
     <row r="28">
       <c r="A28" s="123" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B28" s="124" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C28" s="127" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="D28" s="127"/>
       <c r="E28" s="127"/>
     </row>
     <row r="29">
       <c r="A29" s="123" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B29" s="124" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C29" s="127" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D29" s="127"/>
       <c r="E29" s="127"/>
     </row>
     <row r="30">
       <c r="A30" s="123" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B30" s="124" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C30" s="127" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D30" s="127"/>
       <c r="E30" s="127"/>
     </row>
     <row r="31">
       <c r="A31" s="123" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B31" s="124" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C31" s="127" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="D31" s="127"/>
       <c r="E31" s="127"/>
     </row>
     <row r="32">
       <c r="A32" s="123" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B32" s="124" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C32" s="127" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D32" s="127"/>
       <c r="E32" s="127"/>
     </row>
     <row r="33">
       <c r="A33" s="123" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B33" s="124" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C33" s="127" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D33" s="127"/>
       <c r="E33" s="127"/>
     </row>
     <row r="34">
       <c r="A34" s="123" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B34" s="124" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C34" s="127" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="D34" s="127"/>
       <c r="E34" s="127"/>
     </row>
     <row r="35">
       <c r="A35" s="123" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B35" s="124" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C35" s="127" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D35" s="127"/>
       <c r="E35" s="127"/>
@@ -9664,10 +9675,10 @@
         <v>54.0</v>
       </c>
       <c r="B36" s="131" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C36" s="36" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D36" s="36"/>
       <c r="E36" s="36"/>
@@ -9677,10 +9688,10 @@
         <v>55.0</v>
       </c>
       <c r="B37" s="131" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C37" s="36" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D37" s="36"/>
       <c r="E37" s="36"/>
@@ -9690,10 +9701,10 @@
         <v>56.0</v>
       </c>
       <c r="B38" s="131" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C38" s="36" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D38" s="36"/>
       <c r="E38" s="36"/>
@@ -9703,218 +9714,218 @@
         <v>116.0</v>
       </c>
       <c r="B39" s="131" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C39" s="34" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D39" s="34"/>
       <c r="E39" s="36"/>
     </row>
     <row r="40">
       <c r="A40" s="33" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B40" s="131" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C40" s="34" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D40" s="34"/>
       <c r="E40" s="36"/>
     </row>
     <row r="41">
       <c r="A41" s="33" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B41" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="C41" s="132" t="s">
         <v>112</v>
-      </c>
-      <c r="C41" s="132" t="s">
-        <v>111</v>
       </c>
       <c r="D41" s="132"/>
       <c r="E41" s="36"/>
     </row>
     <row r="42">
       <c r="A42" s="38" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B42" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="C42" s="132" t="s">
         <v>115</v>
-      </c>
-      <c r="C42" s="132" t="s">
-        <v>114</v>
       </c>
       <c r="D42" s="132"/>
       <c r="E42" s="36"/>
     </row>
     <row r="43">
       <c r="A43" s="33" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B43" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="C43" s="132" t="s">
         <v>118</v>
-      </c>
-      <c r="C43" s="132" t="s">
-        <v>117</v>
       </c>
       <c r="D43" s="132"/>
       <c r="E43" s="36"/>
     </row>
     <row r="44">
       <c r="A44" s="38" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B44" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="C44" s="132" t="s">
         <v>121</v>
-      </c>
-      <c r="C44" s="132" t="s">
-        <v>120</v>
       </c>
       <c r="D44" s="132"/>
       <c r="E44" s="36"/>
     </row>
     <row r="45">
       <c r="A45" s="33" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B45" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="C45" s="132" t="s">
         <v>124</v>
-      </c>
-      <c r="C45" s="132" t="s">
-        <v>123</v>
       </c>
       <c r="D45" s="132"/>
       <c r="E45" s="36"/>
     </row>
     <row r="46">
       <c r="A46" s="38" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B46" s="35" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C46" s="132" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="D46" s="132"/>
       <c r="E46" s="36"/>
     </row>
     <row r="47">
       <c r="A47" s="33" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B47" s="35" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C47" s="132" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="D47" s="132"/>
       <c r="E47" s="36"/>
     </row>
     <row r="48">
       <c r="A48" s="38" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B48" s="35" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C48" s="132" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D48" s="132"/>
       <c r="E48" s="36"/>
     </row>
     <row r="49">
       <c r="A49" s="33" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B49" s="35" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C49" s="132" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D49" s="132"/>
       <c r="E49" s="36"/>
     </row>
     <row r="50">
       <c r="A50" s="33" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B50" s="35" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C50" s="132" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="D50" s="132"/>
       <c r="E50" s="36"/>
     </row>
     <row r="51">
       <c r="A51" s="33" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B51" s="35" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C51" s="132" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="D51" s="132"/>
       <c r="E51" s="36"/>
     </row>
     <row r="52">
       <c r="A52" s="33" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B52" s="35" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C52" s="133" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="D52" s="134"/>
       <c r="E52" s="36"/>
     </row>
     <row r="53">
       <c r="A53" s="33" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B53" s="35" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C53" s="133" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="D53" s="135"/>
       <c r="E53" s="36"/>
     </row>
     <row r="54">
       <c r="A54" s="33" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B54" s="35" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C54" s="133" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="D54" s="135"/>
       <c r="E54" s="36"/>
     </row>
     <row r="55">
       <c r="A55" s="38" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C55" s="52" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="D55" s="52"/>
       <c r="E55" s="36"/>
@@ -9950,90 +9961,90 @@
         <v>1</v>
       </c>
       <c r="C1" s="54" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="D1" s="54" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="E1" s="54" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="F1" s="54" t="s">
         <v>10</v>
       </c>
       <c r="G1" s="56" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="13" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F2" s="136"/>
       <c r="G2" s="15"/>
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F3" s="136"/>
       <c r="G3" s="15"/>
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F4" s="136"/>
       <c r="G4" s="15"/>
     </row>
     <row r="5">
       <c r="A5" s="13" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>28</v>
@@ -10043,95 +10054,95 @@
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F6" s="136"/>
       <c r="G6" s="15"/>
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F7" s="136"/>
       <c r="G7" s="15"/>
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F8" s="136"/>
       <c r="G8" s="15"/>
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F9" s="136"/>
       <c r="G9" s="15"/>
     </row>
     <row r="10">
       <c r="A10" s="13" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F10" s="136"/>
       <c r="G10" s="15"/>
@@ -10165,31 +10176,31 @@
         <v>6</v>
       </c>
       <c r="D1" s="54" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D2" s="15"/>
       <c r="F2" s="2" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="12" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D3" s="15"/>
       <c r="F3" s="2" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
   </sheetData>
@@ -10231,19 +10242,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="137" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D1" s="137" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="G1" s="137" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>21</v>
@@ -10252,71 +10263,71 @@
         <v>6</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="K1" s="138" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="C2" s="139"/>
       <c r="D2" s="13"/>
       <c r="G2" s="140"/>
       <c r="I2" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C3" s="140"/>
       <c r="D3" s="13"/>
       <c r="G3" s="140"/>
       <c r="I3" s="2" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="4" ht="20.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="C4" s="140"/>
       <c r="D4" s="13"/>
       <c r="E4" s="141"/>
       <c r="G4" s="142"/>
       <c r="I4" s="2" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="J4" s="143"/>
       <c r="K4" s="2" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C5" s="140"/>
       <c r="D5" s="13"/>
@@ -10324,39 +10335,39 @@
       <c r="F5" s="142"/>
       <c r="G5" s="142"/>
       <c r="I5" s="2" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="J5" s="143"/>
       <c r="K5" s="2" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="6" ht="22.5" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="144"/>
       <c r="G6" s="140"/>
       <c r="I6" s="2" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="7" ht="22.5" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="144"/>
@@ -10364,13 +10375,13 @@
     </row>
     <row r="8" ht="22.5" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="144"/>
@@ -10398,16 +10409,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="32" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
@@ -10423,13 +10434,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
@@ -10470,13 +10481,13 @@
     </row>
     <row r="5">
       <c r="A5" s="15" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -10493,10 +10504,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -10511,10 +10522,10 @@
     <row r="7">
       <c r="A7" s="15"/>
       <c r="B7" s="15" t="s">
+        <v>552</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>551</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>550</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -10529,10 +10540,10 @@
     <row r="8">
       <c r="A8" s="15"/>
       <c r="B8" s="15" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -10547,10 +10558,10 @@
     <row r="9">
       <c r="A9" s="15"/>
       <c r="B9" s="15" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -10578,7 +10589,7 @@
     </row>
     <row r="11">
       <c r="A11" s="15" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B11" s="145" t="s">
         <v>4</v>
@@ -10596,7 +10607,7 @@
     </row>
     <row r="12">
       <c r="A12" s="15" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B12" s="146" t="s">
         <v>3</v>
@@ -10614,10 +10625,10 @@
     </row>
     <row r="13">
       <c r="A13" s="15" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="B13" s="146" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="L13" s="15"/>
     </row>
@@ -10647,38 +10658,38 @@
     </row>
     <row r="20">
       <c r="A20" s="147" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B20" s="148" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="L20" s="15"/>
     </row>
     <row r="21">
       <c r="A21" s="147" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B21" s="148" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="L21" s="15"/>
     </row>
     <row r="22">
       <c r="A22" s="147" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B22" s="149"/>
       <c r="L22" s="15"/>
     </row>
     <row r="23" hidden="1">
       <c r="A23" s="15" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="L23" s="15"/>
     </row>
     <row r="24" hidden="1">
       <c r="A24" s="15" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="L24" s="15"/>
     </row>
@@ -10735,42 +10746,42 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="151" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="C2" s="152" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="153" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="C3" s="152" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="154" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="C4" s="152" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="154" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="C5" s="152" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
spleen fix housingLayers/references confusion
</commit_message>
<xml_diff>
--- a/models/spleen/source/spleen.xlsx
+++ b/models/spleen/source/spleen.xlsx
@@ -8314,12 +8314,11 @@
       <c r="H4" s="15"/>
       <c r="I4" s="12"/>
       <c r="J4" s="20"/>
-      <c r="K4" s="15"/>
+      <c r="K4" s="12" t="s">
+        <v>86</v>
+      </c>
       <c r="L4" s="12" t="s">
         <v>238</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>86</v>
       </c>
       <c r="N4" s="16"/>
       <c r="O4" s="12" t="s">
@@ -8353,12 +8352,11 @@
       <c r="H5" s="15"/>
       <c r="I5" s="12"/>
       <c r="J5" s="20"/>
-      <c r="K5" s="15"/>
+      <c r="K5" s="12" t="s">
+        <v>78</v>
+      </c>
       <c r="L5" s="12" t="s">
         <v>243</v>
-      </c>
-      <c r="M5" s="12" t="s">
-        <v>78</v>
       </c>
       <c r="N5" s="16"/>
       <c r="O5" s="12"/>
@@ -8388,12 +8386,11 @@
       <c r="H6" s="15"/>
       <c r="I6" s="12"/>
       <c r="J6" s="20"/>
-      <c r="K6" s="15"/>
+      <c r="K6" s="12" t="s">
+        <v>78</v>
+      </c>
       <c r="L6" s="12" t="s">
         <v>247</v>
-      </c>
-      <c r="M6" s="12" t="s">
-        <v>78</v>
       </c>
       <c r="N6" s="16"/>
       <c r="O6" s="12"/>
@@ -8422,12 +8419,11 @@
       <c r="H7" s="11"/>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
-      <c r="K7" s="61"/>
+      <c r="K7" s="12" t="s">
+        <v>86</v>
+      </c>
       <c r="L7" s="13" t="s">
         <v>250</v>
-      </c>
-      <c r="M7" s="12" t="s">
-        <v>86</v>
       </c>
       <c r="N7" s="15"/>
       <c r="O7" s="15"/>
@@ -8456,12 +8452,11 @@
       <c r="H8" s="11"/>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
-      <c r="K8" s="61"/>
+      <c r="K8" s="12" t="s">
+        <v>78</v>
+      </c>
       <c r="L8" s="13" t="s">
         <v>254</v>
-      </c>
-      <c r="M8" s="12" t="s">
-        <v>78</v>
       </c>
       <c r="N8" s="15"/>
       <c r="O8" s="15"/>

</xml_diff>